<commit_message>
adjustments to remove duplicates, include NA code
</commit_message>
<xml_diff>
--- a/household-size/data/household-count-by-re-hhsize.xlsx
+++ b/household-size/data/household-count-by-re-hhsize.xlsx
@@ -112,13 +112,13 @@
     <t xml:space="preserve">Some Other Race</t>
   </si>
   <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">Two or More Races</t>
   </si>
   <si>
     <t xml:space="preserve">White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">Multirace PSRC</t>
@@ -958,40 +958,40 @@
         <v>22</v>
       </c>
       <c r="E8" t="n">
-        <v>27739</v>
+        <v>467687</v>
       </c>
       <c r="F8" t="n">
-        <v>27739</v>
+        <v>467139</v>
       </c>
       <c r="G8" t="n">
-        <v>27739</v>
+        <v>467687</v>
       </c>
       <c r="H8" t="n">
-        <v>0.059311034944311</v>
+        <v>0.27614685020285</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0593806126227954</v>
+        <v>0.275933257016484</v>
       </c>
       <c r="J8" t="n">
-        <v>0.059311034944311</v>
+        <v>0.27614685020285</v>
       </c>
       <c r="K8" t="n">
-        <v>1753.3935316929</v>
+        <v>5531.81571257474</v>
       </c>
       <c r="L8" t="n">
-        <v>1753.3935316929</v>
+        <v>5549.62373270736</v>
       </c>
       <c r="M8" t="n">
-        <v>1753.3935316929</v>
+        <v>5531.81571257474</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00371504389479169</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="O8" t="n">
-        <v>0.00372398890528343</v>
+        <v>0.00327260898423871</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00371504389479169</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -1020,40 +1020,40 @@
         <v>22</v>
       </c>
       <c r="E9" t="n">
-        <v>316868</v>
+        <v>27739</v>
       </c>
       <c r="F9" t="n">
-        <v>316527</v>
+        <v>27739</v>
       </c>
       <c r="G9" t="n">
-        <v>316868</v>
+        <v>27739</v>
       </c>
       <c r="H9" t="n">
-        <v>0.677521504767077</v>
+        <v>0.059311034944311</v>
       </c>
       <c r="I9" t="n">
-        <v>0.677586328694457</v>
+        <v>0.0593806126227954</v>
       </c>
       <c r="J9" t="n">
-        <v>0.677521504767077</v>
+        <v>0.059311034944311</v>
       </c>
       <c r="K9" t="n">
-        <v>5104.49905281275</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="L9" t="n">
-        <v>5134.47976547479</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="M9" t="n">
-        <v>5104.49905281275</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00640203655040979</v>
+        <v>0.00371504389479169</v>
       </c>
       <c r="O9" t="n">
-        <v>0.00641730044991988</v>
+        <v>0.00372398890528343</v>
       </c>
       <c r="P9" t="n">
-        <v>0.00640203655040979</v>
+        <v>0.00371504389479169</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -1082,40 +1082,40 @@
         <v>22</v>
       </c>
       <c r="E10" t="n">
-        <v>467687</v>
+        <v>316868</v>
       </c>
       <c r="F10" t="n">
-        <v>467139</v>
+        <v>316527</v>
       </c>
       <c r="G10" t="n">
-        <v>467687</v>
+        <v>316868</v>
       </c>
       <c r="H10" t="n">
-        <v>0.27614685020285</v>
+        <v>0.677521504767077</v>
       </c>
       <c r="I10" t="n">
-        <v>0.275933257016484</v>
+        <v>0.677586328694457</v>
       </c>
       <c r="J10" t="n">
-        <v>0.27614685020285</v>
+        <v>0.677521504767077</v>
       </c>
       <c r="K10" t="n">
-        <v>5531.81571257474</v>
+        <v>5104.49905281275</v>
       </c>
       <c r="L10" t="n">
-        <v>5549.62373270736</v>
+        <v>5134.47976547479</v>
       </c>
       <c r="M10" t="n">
-        <v>5531.81571257474</v>
+        <v>5104.49905281275</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00640203655040979</v>
       </c>
       <c r="O10" t="n">
-        <v>0.00327260898423871</v>
+        <v>0.00641730044991988</v>
       </c>
       <c r="P10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00640203655040979</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -1764,40 +1764,40 @@
         <v>22</v>
       </c>
       <c r="E21" t="n">
-        <v>17552</v>
+        <v>285154</v>
       </c>
       <c r="F21" t="n">
-        <v>17552</v>
+        <v>284882</v>
       </c>
       <c r="G21" t="n">
-        <v>17552</v>
+        <v>285154</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0615527048542191</v>
+        <v>0.307337298897093</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0616114742244157</v>
+        <v>0.307167956767341</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0615527048542191</v>
+        <v>0.307337298897093</v>
       </c>
       <c r="K21" t="n">
-        <v>1504.21367142354</v>
+        <v>4209.61907351589</v>
       </c>
       <c r="L21" t="n">
-        <v>1504.21367142354</v>
+        <v>4187.19517882451</v>
       </c>
       <c r="M21" t="n">
-        <v>1504.21367142354</v>
+        <v>4209.61907351589</v>
       </c>
       <c r="N21" t="n">
-        <v>0.00509752408308916</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="O21" t="n">
-        <v>0.00510862319866652</v>
+        <v>0.00449309450544535</v>
       </c>
       <c r="P21" t="n">
-        <v>0.00509752408308916</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="Q21" t="s">
         <v>23</v>
@@ -1826,40 +1826,40 @@
         <v>22</v>
       </c>
       <c r="E22" t="n">
-        <v>179878</v>
+        <v>17552</v>
       </c>
       <c r="F22" t="n">
-        <v>179654</v>
+        <v>17552</v>
       </c>
       <c r="G22" t="n">
-        <v>179878</v>
+        <v>17552</v>
       </c>
       <c r="H22" t="n">
-        <v>0.630810018446173</v>
+        <v>0.0615527048542191</v>
       </c>
       <c r="I22" t="n">
-        <v>0.630626013577551</v>
+        <v>0.0616114742244157</v>
       </c>
       <c r="J22" t="n">
-        <v>0.630810018446173</v>
+        <v>0.0615527048542191</v>
       </c>
       <c r="K22" t="n">
-        <v>3699.62021384155</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="L22" t="n">
-        <v>3711.27598370106</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="M22" t="n">
-        <v>3699.62021384155</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="N22" t="n">
-        <v>0.00832008151040211</v>
+        <v>0.00509752408308916</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0083894374722481</v>
+        <v>0.00510862319866652</v>
       </c>
       <c r="P22" t="n">
-        <v>0.00832008151040211</v>
+        <v>0.00509752408308916</v>
       </c>
       <c r="Q22" t="s">
         <v>23</v>
@@ -1888,40 +1888,40 @@
         <v>22</v>
       </c>
       <c r="E23" t="n">
-        <v>285154</v>
+        <v>179878</v>
       </c>
       <c r="F23" t="n">
-        <v>284882</v>
+        <v>179654</v>
       </c>
       <c r="G23" t="n">
-        <v>285154</v>
+        <v>179878</v>
       </c>
       <c r="H23" t="n">
-        <v>0.307337298897093</v>
+        <v>0.630810018446173</v>
       </c>
       <c r="I23" t="n">
-        <v>0.307167956767341</v>
+        <v>0.630626013577551</v>
       </c>
       <c r="J23" t="n">
-        <v>0.307337298897093</v>
+        <v>0.630810018446173</v>
       </c>
       <c r="K23" t="n">
-        <v>4209.61907351589</v>
+        <v>3699.62021384155</v>
       </c>
       <c r="L23" t="n">
-        <v>4187.19517882451</v>
+        <v>3711.27598370106</v>
       </c>
       <c r="M23" t="n">
-        <v>4209.61907351589</v>
+        <v>3699.62021384155</v>
       </c>
       <c r="N23" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00832008151040211</v>
       </c>
       <c r="O23" t="n">
-        <v>0.00449309450544535</v>
+        <v>0.0083894374722481</v>
       </c>
       <c r="P23" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00832008151040211</v>
       </c>
       <c r="Q23" t="s">
         <v>23</v>
@@ -2570,40 +2570,40 @@
         <v>22</v>
       </c>
       <c r="E34" t="n">
-        <v>1583</v>
+        <v>25248</v>
       </c>
       <c r="F34" t="n">
-        <v>1583</v>
+        <v>25228</v>
       </c>
       <c r="G34" t="n">
-        <v>1583</v>
+        <v>25248</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0626980354879594</v>
+        <v>0.235381861575179</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0627477406056762</v>
+        <v>0.235239267464847</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0626980354879594</v>
+        <v>0.235381861575179</v>
       </c>
       <c r="K34" t="n">
-        <v>367.183382776917</v>
+        <v>1240.13155872774</v>
       </c>
       <c r="L34" t="n">
-        <v>367.183382776917</v>
+        <v>1245.12493895292</v>
       </c>
       <c r="M34" t="n">
-        <v>367.183382776917</v>
+        <v>1240.13155872774</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0138217730801552</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0138312973780746</v>
+        <v>0.0113265843676149</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0138217730801552</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="Q34" t="s">
         <v>23</v>
@@ -2632,40 +2632,40 @@
         <v>22</v>
       </c>
       <c r="E35" t="n">
-        <v>20362</v>
+        <v>1583</v>
       </c>
       <c r="F35" t="n">
-        <v>20342</v>
+        <v>1583</v>
       </c>
       <c r="G35" t="n">
-        <v>20362</v>
+        <v>1583</v>
       </c>
       <c r="H35" t="n">
-        <v>0.806479721166033</v>
+        <v>0.0626980354879594</v>
       </c>
       <c r="I35" t="n">
-        <v>0.806326304106548</v>
+        <v>0.0627477406056762</v>
       </c>
       <c r="J35" t="n">
-        <v>0.806479721166033</v>
+        <v>0.0626980354879594</v>
       </c>
       <c r="K35" t="n">
-        <v>994.901181410119</v>
+        <v>367.183382776917</v>
       </c>
       <c r="L35" t="n">
-        <v>997.536938408173</v>
+        <v>367.183382776917</v>
       </c>
       <c r="M35" t="n">
-        <v>994.901181410119</v>
+        <v>367.183382776917</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0211425382318378</v>
+        <v>0.0138217730801552</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0211213458731485</v>
+        <v>0.0138312973780746</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0211425382318378</v>
+        <v>0.0138217730801552</v>
       </c>
       <c r="Q35" t="s">
         <v>23</v>
@@ -2694,40 +2694,40 @@
         <v>22</v>
       </c>
       <c r="E36" t="n">
-        <v>25248</v>
+        <v>20362</v>
       </c>
       <c r="F36" t="n">
-        <v>25228</v>
+        <v>20342</v>
       </c>
       <c r="G36" t="n">
-        <v>25248</v>
+        <v>20362</v>
       </c>
       <c r="H36" t="n">
-        <v>0.235381861575179</v>
+        <v>0.806479721166033</v>
       </c>
       <c r="I36" t="n">
-        <v>0.235239267464847</v>
+        <v>0.806326304106548</v>
       </c>
       <c r="J36" t="n">
-        <v>0.235381861575179</v>
+        <v>0.806479721166033</v>
       </c>
       <c r="K36" t="n">
-        <v>1240.13155872774</v>
+        <v>994.901181410119</v>
       </c>
       <c r="L36" t="n">
-        <v>1245.12493895292</v>
+        <v>997.536938408173</v>
       </c>
       <c r="M36" t="n">
-        <v>1240.13155872774</v>
+        <v>994.901181410119</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0211425382318378</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0113265843676149</v>
+        <v>0.0211213458731485</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0211425382318378</v>
       </c>
       <c r="Q36" t="s">
         <v>23</v>
@@ -3376,40 +3376,40 @@
         <v>22</v>
       </c>
       <c r="E47" t="n">
-        <v>5195</v>
+        <v>85103</v>
       </c>
       <c r="F47" t="n">
-        <v>5195</v>
+        <v>84980</v>
       </c>
       <c r="G47" t="n">
-        <v>5195</v>
+        <v>85103</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0610436764861403</v>
+        <v>0.245462280613201</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0611320310661332</v>
+        <v>0.245212187316949</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0610436764861403</v>
+        <v>0.245462280613201</v>
       </c>
       <c r="K47" t="n">
-        <v>800.575802373673</v>
+        <v>2232.66124375598</v>
       </c>
       <c r="L47" t="n">
-        <v>800.575802373673</v>
+        <v>2254.43880155406</v>
       </c>
       <c r="M47" t="n">
-        <v>800.575802373673</v>
+        <v>2232.66124375598</v>
       </c>
       <c r="N47" t="n">
-        <v>0.00950324665414531</v>
+        <v>0.00644852439127257</v>
       </c>
       <c r="O47" t="n">
-        <v>0.00952487560443041</v>
+        <v>0.00649010549686332</v>
       </c>
       <c r="P47" t="n">
-        <v>0.00950324665414531</v>
+        <v>0.00644852439127257</v>
       </c>
       <c r="Q47" t="s">
         <v>23</v>
@@ -3438,40 +3438,40 @@
         <v>22</v>
       </c>
       <c r="E48" t="n">
-        <v>60478</v>
+        <v>5195</v>
       </c>
       <c r="F48" t="n">
-        <v>60405</v>
+        <v>5195</v>
       </c>
       <c r="G48" t="n">
-        <v>60478</v>
+        <v>5195</v>
       </c>
       <c r="H48" t="n">
-        <v>0.710644748128738</v>
+        <v>0.0610436764861403</v>
       </c>
       <c r="I48" t="n">
-        <v>0.710814309249235</v>
+        <v>0.0611320310661332</v>
       </c>
       <c r="J48" t="n">
-        <v>0.710644748128738</v>
+        <v>0.0610436764861403</v>
       </c>
       <c r="K48" t="n">
-        <v>2114.73464289524</v>
+        <v>800.575802373673</v>
       </c>
       <c r="L48" t="n">
-        <v>2130.04494163151</v>
+        <v>800.575802373673</v>
       </c>
       <c r="M48" t="n">
-        <v>2114.73464289524</v>
+        <v>800.575802373673</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0153635742182986</v>
+        <v>0.00950324665414531</v>
       </c>
       <c r="O48" t="n">
-        <v>0.0154265494221258</v>
+        <v>0.00952487560443041</v>
       </c>
       <c r="P48" t="n">
-        <v>0.0153635742182986</v>
+        <v>0.00950324665414531</v>
       </c>
       <c r="Q48" t="s">
         <v>23</v>
@@ -3500,40 +3500,40 @@
         <v>22</v>
       </c>
       <c r="E49" t="n">
-        <v>85103</v>
+        <v>60478</v>
       </c>
       <c r="F49" t="n">
-        <v>84980</v>
+        <v>60405</v>
       </c>
       <c r="G49" t="n">
-        <v>85103</v>
+        <v>60478</v>
       </c>
       <c r="H49" t="n">
-        <v>0.245462280613201</v>
+        <v>0.710644748128738</v>
       </c>
       <c r="I49" t="n">
-        <v>0.245212187316949</v>
+        <v>0.710814309249235</v>
       </c>
       <c r="J49" t="n">
-        <v>0.245462280613201</v>
+        <v>0.710644748128738</v>
       </c>
       <c r="K49" t="n">
-        <v>2232.66124375598</v>
+        <v>2114.73464289524</v>
       </c>
       <c r="L49" t="n">
-        <v>2254.43880155406</v>
+        <v>2130.04494163151</v>
       </c>
       <c r="M49" t="n">
-        <v>2232.66124375598</v>
+        <v>2114.73464289524</v>
       </c>
       <c r="N49" t="n">
-        <v>0.00644852439127257</v>
+        <v>0.0153635742182986</v>
       </c>
       <c r="O49" t="n">
-        <v>0.00649010549686332</v>
+        <v>0.0154265494221258</v>
       </c>
       <c r="P49" t="n">
-        <v>0.00644852439127257</v>
+        <v>0.0153635742182986</v>
       </c>
       <c r="Q49" t="s">
         <v>23</v>
@@ -4182,40 +4182,40 @@
         <v>22</v>
       </c>
       <c r="E60" t="n">
-        <v>3409</v>
+        <v>72182</v>
       </c>
       <c r="F60" t="n">
-        <v>3409</v>
+        <v>72049</v>
       </c>
       <c r="G60" t="n">
-        <v>3409</v>
+        <v>72182</v>
       </c>
       <c r="H60" t="n">
-        <v>0.0472278407359175</v>
+        <v>0.231480917303505</v>
       </c>
       <c r="I60" t="n">
-        <v>0.0473150217213285</v>
+        <v>0.23115298979127</v>
       </c>
       <c r="J60" t="n">
-        <v>0.0472278407359175</v>
+        <v>0.231480917303505</v>
       </c>
       <c r="K60" t="n">
-        <v>592.233927153156</v>
+        <v>2455.15607980735</v>
       </c>
       <c r="L60" t="n">
-        <v>592.233927153156</v>
+        <v>2439.55895942381</v>
       </c>
       <c r="M60" t="n">
-        <v>592.233927153156</v>
+        <v>2455.15607980735</v>
       </c>
       <c r="N60" t="n">
-        <v>0.00820392037282418</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="O60" t="n">
-        <v>0.00821430188089977</v>
+        <v>0.00774704176324199</v>
       </c>
       <c r="P60" t="n">
-        <v>0.00820392037282418</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="Q60" t="s">
         <v>23</v>
@@ -4244,40 +4244,40 @@
         <v>22</v>
       </c>
       <c r="E61" t="n">
-        <v>56150</v>
+        <v>3409</v>
       </c>
       <c r="F61" t="n">
-        <v>56126</v>
+        <v>3409</v>
       </c>
       <c r="G61" t="n">
-        <v>56150</v>
+        <v>3409</v>
       </c>
       <c r="H61" t="n">
-        <v>0.777894766008146</v>
+        <v>0.0472278407359175</v>
       </c>
       <c r="I61" t="n">
-        <v>0.77899762661522</v>
+        <v>0.0473150217213285</v>
       </c>
       <c r="J61" t="n">
-        <v>0.777894766008146</v>
+        <v>0.0472278407359175</v>
       </c>
       <c r="K61" t="n">
-        <v>1998.48601915206</v>
+        <v>592.233927153156</v>
       </c>
       <c r="L61" t="n">
-        <v>2000.98194886161</v>
+        <v>592.233927153156</v>
       </c>
       <c r="M61" t="n">
-        <v>1998.48601915206</v>
+        <v>592.233927153156</v>
       </c>
       <c r="N61" t="n">
-        <v>0.0153151457594137</v>
+        <v>0.00820392037282418</v>
       </c>
       <c r="O61" t="n">
-        <v>0.0152087577905497</v>
+        <v>0.00821430188089977</v>
       </c>
       <c r="P61" t="n">
-        <v>0.0153151457594137</v>
+        <v>0.00820392037282418</v>
       </c>
       <c r="Q61" t="s">
         <v>23</v>
@@ -4306,40 +4306,40 @@
         <v>22</v>
       </c>
       <c r="E62" t="n">
-        <v>72182</v>
+        <v>56150</v>
       </c>
       <c r="F62" t="n">
-        <v>72049</v>
+        <v>56126</v>
       </c>
       <c r="G62" t="n">
-        <v>72182</v>
+        <v>56150</v>
       </c>
       <c r="H62" t="n">
-        <v>0.231480917303505</v>
+        <v>0.777894766008146</v>
       </c>
       <c r="I62" t="n">
-        <v>0.23115298979127</v>
+        <v>0.77899762661522</v>
       </c>
       <c r="J62" t="n">
-        <v>0.231480917303505</v>
+        <v>0.777894766008146</v>
       </c>
       <c r="K62" t="n">
-        <v>2455.15607980735</v>
+        <v>1998.48601915206</v>
       </c>
       <c r="L62" t="n">
-        <v>2439.55895942381</v>
+        <v>2000.98194886161</v>
       </c>
       <c r="M62" t="n">
-        <v>2455.15607980735</v>
+        <v>1998.48601915206</v>
       </c>
       <c r="N62" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.0153151457594137</v>
       </c>
       <c r="O62" t="n">
-        <v>0.00774704176324199</v>
+        <v>0.0152087577905497</v>
       </c>
       <c r="P62" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.0153151457594137</v>
       </c>
       <c r="Q62" t="s">
         <v>23</v>
@@ -5064,40 +5064,40 @@
         <v>22</v>
       </c>
       <c r="E8" t="n">
-        <v>65735</v>
+        <v>1225930</v>
       </c>
       <c r="F8" t="n">
-        <v>22627</v>
+        <v>1225803</v>
       </c>
       <c r="G8" t="n">
-        <v>20365</v>
+        <v>1225930</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0536205166689778</v>
+        <v>0.72385314979715</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0184589203974864</v>
+        <v>0.724066742983516</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0166118783291053</v>
+        <v>0.72385314979715</v>
       </c>
       <c r="K8" t="n">
-        <v>2474.29871298895</v>
+        <v>6292.05513549448</v>
       </c>
       <c r="L8" t="n">
-        <v>1662.96311816363</v>
+        <v>6298.22140556721</v>
       </c>
       <c r="M8" t="n">
-        <v>1455.59974768693</v>
+        <v>6292.05513549448</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00200596629495626</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="O8" t="n">
-        <v>0.00135780707407631</v>
+        <v>0.00327260898423871</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00119130073452516</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -5126,40 +5126,40 @@
         <v>22</v>
       </c>
       <c r="E9" t="n">
-        <v>793881</v>
+        <v>65735</v>
       </c>
       <c r="F9" t="n">
-        <v>655535</v>
+        <v>22627</v>
       </c>
       <c r="G9" t="n">
-        <v>636168</v>
+        <v>20365</v>
       </c>
       <c r="H9" t="n">
-        <v>0.647574494465426</v>
+        <v>0.0536205166689778</v>
       </c>
       <c r="I9" t="n">
-        <v>0.534780058459638</v>
+        <v>0.0184589203974864</v>
       </c>
       <c r="J9" t="n">
-        <v>0.518926855530087</v>
+        <v>0.0166118783291053</v>
       </c>
       <c r="K9" t="n">
-        <v>5814.84224063871</v>
+        <v>2474.29871298895</v>
       </c>
       <c r="L9" t="n">
-        <v>5060.82232845809</v>
+        <v>1662.96311816363</v>
       </c>
       <c r="M9" t="n">
-        <v>5119.44603051822</v>
+        <v>1455.59974768693</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00297386642019264</v>
+        <v>0.00200596629495626</v>
       </c>
       <c r="O9" t="n">
-        <v>0.00274427536456074</v>
+        <v>0.00135780707407631</v>
       </c>
       <c r="P9" t="n">
-        <v>0.00299876214304256</v>
+        <v>0.00119130073452516</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -5188,40 +5188,40 @@
         <v>22</v>
       </c>
       <c r="E10" t="n">
-        <v>1225930</v>
+        <v>793881</v>
       </c>
       <c r="F10" t="n">
-        <v>1225803</v>
+        <v>655535</v>
       </c>
       <c r="G10" t="n">
-        <v>1225930</v>
+        <v>636168</v>
       </c>
       <c r="H10" t="n">
-        <v>0.72385314979715</v>
+        <v>0.647574494465426</v>
       </c>
       <c r="I10" t="n">
-        <v>0.724066742983516</v>
+        <v>0.534780058459638</v>
       </c>
       <c r="J10" t="n">
-        <v>0.72385314979715</v>
+        <v>0.518926855530087</v>
       </c>
       <c r="K10" t="n">
-        <v>6292.05513549448</v>
+        <v>5814.84224063871</v>
       </c>
       <c r="L10" t="n">
-        <v>6298.22140556721</v>
+        <v>5060.82232845809</v>
       </c>
       <c r="M10" t="n">
-        <v>6292.05513549448</v>
+        <v>5119.44603051822</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00297386642019264</v>
       </c>
       <c r="O10" t="n">
-        <v>0.00327260898423871</v>
+        <v>0.00274427536456074</v>
       </c>
       <c r="P10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00299876214304256</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -6130,40 +6130,40 @@
         <v>22</v>
       </c>
       <c r="E26" t="n">
-        <v>31925</v>
+        <v>642667</v>
       </c>
       <c r="F26" t="n">
-        <v>10640</v>
+        <v>642565</v>
       </c>
       <c r="G26" t="n">
-        <v>9604</v>
+        <v>642667</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0496758041100601</v>
+        <v>0.692662701102907</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0165586360912904</v>
+        <v>0.692832043232659</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0149439756514649</v>
+        <v>0.692662701102907</v>
       </c>
       <c r="K26" t="n">
-        <v>1887.26567187525</v>
+        <v>4626.22104388858</v>
       </c>
       <c r="L26" t="n">
-        <v>1337.34554369841</v>
+        <v>4628.15173571346</v>
       </c>
       <c r="M26" t="n">
-        <v>1108.47980485663</v>
+        <v>4626.22104388858</v>
       </c>
       <c r="N26" t="n">
-        <v>0.0029246552583609</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="O26" t="n">
-        <v>0.00206847613429708</v>
+        <v>0.00449309450544533</v>
       </c>
       <c r="P26" t="n">
-        <v>0.00171185706555702</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="Q26" t="s">
         <v>23</v>
@@ -6192,40 +6192,40 @@
         <v>22</v>
       </c>
       <c r="E27" t="n">
-        <v>383636</v>
+        <v>31925</v>
       </c>
       <c r="F27" t="n">
-        <v>311212</v>
+        <v>10640</v>
       </c>
       <c r="G27" t="n">
-        <v>304101</v>
+        <v>9604</v>
       </c>
       <c r="H27" t="n">
-        <v>0.596943673784402</v>
+        <v>0.0496758041100601</v>
       </c>
       <c r="I27" t="n">
-        <v>0.484327655567919</v>
+        <v>0.0165586360912904</v>
       </c>
       <c r="J27" t="n">
-        <v>0.473185957891101</v>
+        <v>0.0149439756514649</v>
       </c>
       <c r="K27" t="n">
-        <v>4095.13287589014</v>
+        <v>1887.26567187525</v>
       </c>
       <c r="L27" t="n">
-        <v>3369.53323132244</v>
+        <v>1337.34554369841</v>
       </c>
       <c r="M27" t="n">
-        <v>3472.84881243213</v>
+        <v>1108.47980485663</v>
       </c>
       <c r="N27" t="n">
-        <v>0.00430134638534656</v>
+        <v>0.0029246552583609</v>
       </c>
       <c r="O27" t="n">
-        <v>0.00366948826611233</v>
+        <v>0.00206847613429708</v>
       </c>
       <c r="P27" t="n">
-        <v>0.00394456144798949</v>
+        <v>0.00171185706555702</v>
       </c>
       <c r="Q27" t="s">
         <v>23</v>
@@ -6254,40 +6254,40 @@
         <v>22</v>
       </c>
       <c r="E28" t="n">
-        <v>642667</v>
+        <v>383636</v>
       </c>
       <c r="F28" t="n">
-        <v>642565</v>
+        <v>311212</v>
       </c>
       <c r="G28" t="n">
-        <v>642667</v>
+        <v>304101</v>
       </c>
       <c r="H28" t="n">
-        <v>0.692662701102907</v>
+        <v>0.596943673784402</v>
       </c>
       <c r="I28" t="n">
-        <v>0.692832043232659</v>
+        <v>0.484327655567919</v>
       </c>
       <c r="J28" t="n">
-        <v>0.692662701102907</v>
+        <v>0.473185957891101</v>
       </c>
       <c r="K28" t="n">
-        <v>4626.22104388858</v>
+        <v>4095.13287589014</v>
       </c>
       <c r="L28" t="n">
-        <v>4628.15173571346</v>
+        <v>3369.53323132244</v>
       </c>
       <c r="M28" t="n">
-        <v>4626.22104388858</v>
+        <v>3472.84881243213</v>
       </c>
       <c r="N28" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00430134638534656</v>
       </c>
       <c r="O28" t="n">
-        <v>0.00449309450544533</v>
+        <v>0.00366948826611233</v>
       </c>
       <c r="P28" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00394456144798949</v>
       </c>
       <c r="Q28" t="s">
         <v>23</v>
@@ -7196,40 +7196,40 @@
         <v>22</v>
       </c>
       <c r="E44" t="n">
-        <v>4170</v>
+        <v>82016</v>
       </c>
       <c r="F44" t="n">
-        <v>1523</v>
+        <v>82016</v>
       </c>
       <c r="G44" t="n">
-        <v>1384</v>
+        <v>82016</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0508437378072571</v>
+        <v>0.764618138424821</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0185695474053843</v>
+        <v>0.764760732535154</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0168747561451424</v>
+        <v>0.764618138424821</v>
       </c>
       <c r="K44" t="n">
-        <v>524.416092754599</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="L44" t="n">
-        <v>299.792844360902</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="M44" t="n">
-        <v>286.149865937851</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="N44" t="n">
-        <v>0.00633768612955597</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0036574132905182</v>
+        <v>0.0113265843676149</v>
       </c>
       <c r="P44" t="n">
-        <v>0.00347463222320292</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="Q44" t="s">
         <v>23</v>
@@ -7258,40 +7258,40 @@
         <v>22</v>
       </c>
       <c r="E45" t="n">
-        <v>64736</v>
+        <v>4170</v>
       </c>
       <c r="F45" t="n">
-        <v>54991</v>
+        <v>1523</v>
       </c>
       <c r="G45" t="n">
-        <v>53126</v>
+        <v>1384</v>
       </c>
       <c r="H45" t="n">
-        <v>0.789309403043309</v>
+        <v>0.0508437378072571</v>
       </c>
       <c r="I45" t="n">
-        <v>0.670491123683184</v>
+        <v>0.0185695474053843</v>
       </c>
       <c r="J45" t="n">
-        <v>0.647751658213032</v>
+        <v>0.0168747561451424</v>
       </c>
       <c r="K45" t="n">
-        <v>1210.94979765523</v>
+        <v>524.416092754599</v>
       </c>
       <c r="L45" t="n">
-        <v>1240.6277659818</v>
+        <v>299.792844360902</v>
       </c>
       <c r="M45" t="n">
-        <v>1208.74936924544</v>
+        <v>286.149865937851</v>
       </c>
       <c r="N45" t="n">
-        <v>0.00931194669267898</v>
+        <v>0.00633768612955597</v>
       </c>
       <c r="O45" t="n">
-        <v>0.0113234610137819</v>
+        <v>0.0036574132905182</v>
       </c>
       <c r="P45" t="n">
-        <v>0.0112307730915826</v>
+        <v>0.00347463222320292</v>
       </c>
       <c r="Q45" t="s">
         <v>23</v>
@@ -7320,40 +7320,40 @@
         <v>22</v>
       </c>
       <c r="E46" t="n">
-        <v>82016</v>
+        <v>64736</v>
       </c>
       <c r="F46" t="n">
-        <v>82016</v>
+        <v>54991</v>
       </c>
       <c r="G46" t="n">
-        <v>82016</v>
+        <v>53126</v>
       </c>
       <c r="H46" t="n">
-        <v>0.764618138424821</v>
+        <v>0.789309403043309</v>
       </c>
       <c r="I46" t="n">
-        <v>0.764760732535154</v>
+        <v>0.670491123683184</v>
       </c>
       <c r="J46" t="n">
-        <v>0.764618138424821</v>
+        <v>0.647751658213032</v>
       </c>
       <c r="K46" t="n">
-        <v>1309.15839613519</v>
+        <v>1210.94979765523</v>
       </c>
       <c r="L46" t="n">
-        <v>1309.15839613519</v>
+        <v>1240.6277659818</v>
       </c>
       <c r="M46" t="n">
-        <v>1309.15839613519</v>
+        <v>1208.74936924544</v>
       </c>
       <c r="N46" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.00931194669267898</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0113265843676149</v>
+        <v>0.0113234610137819</v>
       </c>
       <c r="P46" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0112307730915826</v>
       </c>
       <c r="Q46" t="s">
         <v>23</v>
@@ -8262,40 +8262,40 @@
         <v>22</v>
       </c>
       <c r="E62" t="n">
-        <v>18750</v>
+        <v>261602</v>
       </c>
       <c r="F62" t="n">
-        <v>6495</v>
+        <v>261577</v>
       </c>
       <c r="G62" t="n">
-        <v>5686</v>
+        <v>261602</v>
       </c>
       <c r="H62" t="n">
-        <v>0.0716737639620492</v>
+        <v>0.754537719386799</v>
       </c>
       <c r="I62" t="n">
-        <v>0.0248301647316087</v>
+        <v>0.754787812683051</v>
       </c>
       <c r="J62" t="n">
-        <v>0.021735307834038</v>
+        <v>0.754537719386799</v>
       </c>
       <c r="K62" t="n">
-        <v>1242.4073636488</v>
+        <v>2501.32257198692</v>
       </c>
       <c r="L62" t="n">
-        <v>809.74930757766</v>
+        <v>2500.28720132083</v>
       </c>
       <c r="M62" t="n">
-        <v>712.80851027292</v>
+        <v>2501.32257198692</v>
       </c>
       <c r="N62" t="n">
-        <v>0.00471669847814188</v>
+        <v>0.00644852439127255</v>
       </c>
       <c r="O62" t="n">
-        <v>0.00310336492896555</v>
+        <v>0.00649010549686331</v>
       </c>
       <c r="P62" t="n">
-        <v>0.0027395071922153</v>
+        <v>0.00644852439127255</v>
       </c>
       <c r="Q62" t="s">
         <v>23</v>
@@ -8324,40 +8324,40 @@
         <v>22</v>
       </c>
       <c r="E63" t="n">
-        <v>179301</v>
+        <v>18750</v>
       </c>
       <c r="F63" t="n">
-        <v>147690</v>
+        <v>6495</v>
       </c>
       <c r="G63" t="n">
-        <v>141989</v>
+        <v>5686</v>
       </c>
       <c r="H63" t="n">
-        <v>0.685396136115167</v>
+        <v>0.0716737639620492</v>
       </c>
       <c r="I63" t="n">
-        <v>0.564613861310436</v>
+        <v>0.0248301647316087</v>
       </c>
       <c r="J63" t="n">
-        <v>0.542767257131062</v>
+        <v>0.021735307834038</v>
       </c>
       <c r="K63" t="n">
-        <v>2122.68338987206</v>
+        <v>1242.4073636488</v>
       </c>
       <c r="L63" t="n">
-        <v>1811.25884655811</v>
+        <v>809.74930757766</v>
       </c>
       <c r="M63" t="n">
-        <v>1895.27634691521</v>
+        <v>712.80851027292</v>
       </c>
       <c r="N63" t="n">
-        <v>0.00612002931455315</v>
+        <v>0.00471669847814188</v>
       </c>
       <c r="O63" t="n">
-        <v>0.0053294207179917</v>
+        <v>0.00310336492896555</v>
       </c>
       <c r="P63" t="n">
-        <v>0.0061204535387096</v>
+        <v>0.0027395071922153</v>
       </c>
       <c r="Q63" t="s">
         <v>23</v>
@@ -8386,40 +8386,40 @@
         <v>22</v>
       </c>
       <c r="E64" t="n">
-        <v>261602</v>
+        <v>179301</v>
       </c>
       <c r="F64" t="n">
-        <v>261577</v>
+        <v>147690</v>
       </c>
       <c r="G64" t="n">
-        <v>261602</v>
+        <v>141989</v>
       </c>
       <c r="H64" t="n">
-        <v>0.754537719386799</v>
+        <v>0.685396136115167</v>
       </c>
       <c r="I64" t="n">
-        <v>0.754787812683051</v>
+        <v>0.564613861310436</v>
       </c>
       <c r="J64" t="n">
-        <v>0.754537719386799</v>
+        <v>0.542767257131062</v>
       </c>
       <c r="K64" t="n">
-        <v>2501.32257198692</v>
+        <v>2122.68338987206</v>
       </c>
       <c r="L64" t="n">
-        <v>2500.28720132083</v>
+        <v>1811.25884655811</v>
       </c>
       <c r="M64" t="n">
-        <v>2501.32257198692</v>
+        <v>1895.27634691521</v>
       </c>
       <c r="N64" t="n">
-        <v>0.00644852439127255</v>
+        <v>0.00612002931455315</v>
       </c>
       <c r="O64" t="n">
-        <v>0.00649010549686331</v>
+        <v>0.0053294207179917</v>
       </c>
       <c r="P64" t="n">
-        <v>0.00644852439127255</v>
+        <v>0.0061204535387096</v>
       </c>
       <c r="Q64" t="s">
         <v>23</v>
@@ -9328,40 +9328,40 @@
         <v>22</v>
       </c>
       <c r="E80" t="n">
-        <v>10890</v>
+        <v>239645</v>
       </c>
       <c r="F80" t="n">
-        <v>3969</v>
+        <v>239645</v>
       </c>
       <c r="G80" t="n">
-        <v>3691</v>
+        <v>239645</v>
       </c>
       <c r="H80" t="n">
-        <v>0.045442216612072</v>
+        <v>0.768519082696495</v>
       </c>
       <c r="I80" t="n">
-        <v>0.0165619979553089</v>
+        <v>0.76884701020873</v>
       </c>
       <c r="J80" t="n">
-        <v>0.0154019487158088</v>
+        <v>0.768519082696495</v>
       </c>
       <c r="K80" t="n">
-        <v>847.453087125624</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="L80" t="n">
-        <v>607.97428572679</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="M80" t="n">
-        <v>616.82608672745</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="N80" t="n">
-        <v>0.00356500723312259</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="O80" t="n">
-        <v>0.002539866097422</v>
+        <v>0.00774704176324198</v>
       </c>
       <c r="P80" t="n">
-        <v>0.00257712385489421</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="Q80" t="s">
         <v>23</v>
@@ -9390,40 +9390,40 @@
         <v>22</v>
       </c>
       <c r="E81" t="n">
-        <v>166208</v>
+        <v>10890</v>
       </c>
       <c r="F81" t="n">
-        <v>141642</v>
+        <v>3969</v>
       </c>
       <c r="G81" t="n">
-        <v>136952</v>
+        <v>3691</v>
       </c>
       <c r="H81" t="n">
-        <v>0.69355922301738</v>
+        <v>0.045442216612072</v>
       </c>
       <c r="I81" t="n">
-        <v>0.591049260364289</v>
+        <v>0.0165619979553089</v>
       </c>
       <c r="J81" t="n">
-        <v>0.571478645496464</v>
+        <v>0.0154019487158088</v>
       </c>
       <c r="K81" t="n">
-        <v>2287.87585247375</v>
+        <v>847.453087125624</v>
       </c>
       <c r="L81" t="n">
-        <v>2107.858318533</v>
+        <v>607.97428572679</v>
       </c>
       <c r="M81" t="n">
-        <v>1957.33924894932</v>
+        <v>616.82608672745</v>
       </c>
       <c r="N81" t="n">
-        <v>0.00607006523918823</v>
+        <v>0.00356500723312259</v>
       </c>
       <c r="O81" t="n">
-        <v>0.00539918277279873</v>
+        <v>0.002539866097422</v>
       </c>
       <c r="P81" t="n">
-        <v>0.00555214543106352</v>
+        <v>0.00257712385489421</v>
       </c>
       <c r="Q81" t="s">
         <v>23</v>
@@ -9452,40 +9452,40 @@
         <v>22</v>
       </c>
       <c r="E82" t="n">
-        <v>239645</v>
+        <v>166208</v>
       </c>
       <c r="F82" t="n">
-        <v>239645</v>
+        <v>141642</v>
       </c>
       <c r="G82" t="n">
-        <v>239645</v>
+        <v>136952</v>
       </c>
       <c r="H82" t="n">
-        <v>0.768519082696495</v>
+        <v>0.69355922301738</v>
       </c>
       <c r="I82" t="n">
-        <v>0.76884701020873</v>
+        <v>0.591049260364289</v>
       </c>
       <c r="J82" t="n">
-        <v>0.768519082696495</v>
+        <v>0.571478645496464</v>
       </c>
       <c r="K82" t="n">
-        <v>2556.52132729956</v>
+        <v>2287.87585247375</v>
       </c>
       <c r="L82" t="n">
-        <v>2556.52132729956</v>
+        <v>2107.858318533</v>
       </c>
       <c r="M82" t="n">
-        <v>2556.52132729956</v>
+        <v>1957.33924894932</v>
       </c>
       <c r="N82" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.00607006523918823</v>
       </c>
       <c r="O82" t="n">
-        <v>0.00774704176324198</v>
+        <v>0.00539918277279873</v>
       </c>
       <c r="P82" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.00555214543106352</v>
       </c>
       <c r="Q82" t="s">
         <v>23</v>
@@ -10470,40 +10470,40 @@
         <v>50</v>
       </c>
       <c r="E8" t="n">
-        <v>27739</v>
+        <v>467687</v>
       </c>
       <c r="F8" t="n">
-        <v>27739</v>
+        <v>467139</v>
       </c>
       <c r="G8" t="n">
-        <v>27739</v>
+        <v>467687</v>
       </c>
       <c r="H8" t="n">
-        <v>0.059311034944311</v>
+        <v>0.27614685020285</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0593806126227954</v>
+        <v>0.275933257016484</v>
       </c>
       <c r="J8" t="n">
-        <v>0.059311034944311</v>
+        <v>0.27614685020285</v>
       </c>
       <c r="K8" t="n">
-        <v>1753.3935316929</v>
+        <v>5531.81571257474</v>
       </c>
       <c r="L8" t="n">
-        <v>1753.3935316929</v>
+        <v>5549.62373270736</v>
       </c>
       <c r="M8" t="n">
-        <v>1753.3935316929</v>
+        <v>5531.81571257474</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00371504389479169</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="O8" t="n">
-        <v>0.00372398890528343</v>
+        <v>0.00327260898423871</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00371504389479169</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -10532,40 +10532,40 @@
         <v>50</v>
       </c>
       <c r="E9" t="n">
-        <v>316868</v>
+        <v>27739</v>
       </c>
       <c r="F9" t="n">
-        <v>316527</v>
+        <v>27739</v>
       </c>
       <c r="G9" t="n">
-        <v>316868</v>
+        <v>27739</v>
       </c>
       <c r="H9" t="n">
-        <v>0.677521504767077</v>
+        <v>0.059311034944311</v>
       </c>
       <c r="I9" t="n">
-        <v>0.677586328694457</v>
+        <v>0.0593806126227954</v>
       </c>
       <c r="J9" t="n">
-        <v>0.677521504767077</v>
+        <v>0.059311034944311</v>
       </c>
       <c r="K9" t="n">
-        <v>5104.49905281275</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="L9" t="n">
-        <v>5134.47976547479</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="M9" t="n">
-        <v>5104.49905281275</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00640203655040979</v>
+        <v>0.00371504389479169</v>
       </c>
       <c r="O9" t="n">
-        <v>0.00641730044991988</v>
+        <v>0.00372398890528343</v>
       </c>
       <c r="P9" t="n">
-        <v>0.00640203655040979</v>
+        <v>0.00371504389479169</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -10594,40 +10594,40 @@
         <v>50</v>
       </c>
       <c r="E10" t="n">
-        <v>467687</v>
+        <v>316868</v>
       </c>
       <c r="F10" t="n">
-        <v>467139</v>
+        <v>316527</v>
       </c>
       <c r="G10" t="n">
-        <v>467687</v>
+        <v>316868</v>
       </c>
       <c r="H10" t="n">
-        <v>0.27614685020285</v>
+        <v>0.677521504767077</v>
       </c>
       <c r="I10" t="n">
-        <v>0.275933257016484</v>
+        <v>0.677586328694457</v>
       </c>
       <c r="J10" t="n">
-        <v>0.27614685020285</v>
+        <v>0.677521504767077</v>
       </c>
       <c r="K10" t="n">
-        <v>5531.81571257474</v>
+        <v>5104.49905281275</v>
       </c>
       <c r="L10" t="n">
-        <v>5549.62373270736</v>
+        <v>5134.47976547479</v>
       </c>
       <c r="M10" t="n">
-        <v>5531.81571257474</v>
+        <v>5104.49905281275</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00640203655040979</v>
       </c>
       <c r="O10" t="n">
-        <v>0.00327260898423871</v>
+        <v>0.00641730044991988</v>
       </c>
       <c r="P10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00640203655040979</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -11276,40 +11276,40 @@
         <v>50</v>
       </c>
       <c r="E21" t="n">
-        <v>17552</v>
+        <v>285154</v>
       </c>
       <c r="F21" t="n">
-        <v>17552</v>
+        <v>284882</v>
       </c>
       <c r="G21" t="n">
-        <v>17552</v>
+        <v>285154</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0615527048542191</v>
+        <v>0.307337298897093</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0616114742244157</v>
+        <v>0.307167956767341</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0615527048542191</v>
+        <v>0.307337298897093</v>
       </c>
       <c r="K21" t="n">
-        <v>1504.21367142354</v>
+        <v>4209.61907351589</v>
       </c>
       <c r="L21" t="n">
-        <v>1504.21367142354</v>
+        <v>4187.19517882451</v>
       </c>
       <c r="M21" t="n">
-        <v>1504.21367142354</v>
+        <v>4209.61907351589</v>
       </c>
       <c r="N21" t="n">
-        <v>0.00509752408308916</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="O21" t="n">
-        <v>0.00510862319866652</v>
+        <v>0.00449309450544535</v>
       </c>
       <c r="P21" t="n">
-        <v>0.00509752408308916</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="Q21" t="s">
         <v>23</v>
@@ -11338,40 +11338,40 @@
         <v>50</v>
       </c>
       <c r="E22" t="n">
-        <v>179878</v>
+        <v>17552</v>
       </c>
       <c r="F22" t="n">
-        <v>179654</v>
+        <v>17552</v>
       </c>
       <c r="G22" t="n">
-        <v>179878</v>
+        <v>17552</v>
       </c>
       <c r="H22" t="n">
-        <v>0.630810018446173</v>
+        <v>0.0615527048542191</v>
       </c>
       <c r="I22" t="n">
-        <v>0.630626013577551</v>
+        <v>0.0616114742244157</v>
       </c>
       <c r="J22" t="n">
-        <v>0.630810018446173</v>
+        <v>0.0615527048542191</v>
       </c>
       <c r="K22" t="n">
-        <v>3699.62021384155</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="L22" t="n">
-        <v>3711.27598370106</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="M22" t="n">
-        <v>3699.62021384155</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="N22" t="n">
-        <v>0.00832008151040211</v>
+        <v>0.00509752408308916</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0083894374722481</v>
+        <v>0.00510862319866652</v>
       </c>
       <c r="P22" t="n">
-        <v>0.00832008151040211</v>
+        <v>0.00509752408308916</v>
       </c>
       <c r="Q22" t="s">
         <v>23</v>
@@ -11400,40 +11400,40 @@
         <v>50</v>
       </c>
       <c r="E23" t="n">
-        <v>285154</v>
+        <v>179878</v>
       </c>
       <c r="F23" t="n">
-        <v>284882</v>
+        <v>179654</v>
       </c>
       <c r="G23" t="n">
-        <v>285154</v>
+        <v>179878</v>
       </c>
       <c r="H23" t="n">
-        <v>0.307337298897093</v>
+        <v>0.630810018446173</v>
       </c>
       <c r="I23" t="n">
-        <v>0.307167956767341</v>
+        <v>0.630626013577551</v>
       </c>
       <c r="J23" t="n">
-        <v>0.307337298897093</v>
+        <v>0.630810018446173</v>
       </c>
       <c r="K23" t="n">
-        <v>4209.61907351589</v>
+        <v>3699.62021384155</v>
       </c>
       <c r="L23" t="n">
-        <v>4187.19517882451</v>
+        <v>3711.27598370106</v>
       </c>
       <c r="M23" t="n">
-        <v>4209.61907351589</v>
+        <v>3699.62021384155</v>
       </c>
       <c r="N23" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00832008151040211</v>
       </c>
       <c r="O23" t="n">
-        <v>0.00449309450544535</v>
+        <v>0.0083894374722481</v>
       </c>
       <c r="P23" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00832008151040211</v>
       </c>
       <c r="Q23" t="s">
         <v>23</v>
@@ -12082,40 +12082,40 @@
         <v>50</v>
       </c>
       <c r="E34" t="n">
-        <v>1583</v>
+        <v>25248</v>
       </c>
       <c r="F34" t="n">
-        <v>1583</v>
+        <v>25228</v>
       </c>
       <c r="G34" t="n">
-        <v>1583</v>
+        <v>25248</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0626980354879594</v>
+        <v>0.235381861575179</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0627477406056762</v>
+        <v>0.235239267464847</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0626980354879594</v>
+        <v>0.235381861575179</v>
       </c>
       <c r="K34" t="n">
-        <v>367.183382776917</v>
+        <v>1240.13155872774</v>
       </c>
       <c r="L34" t="n">
-        <v>367.183382776917</v>
+        <v>1245.12493895292</v>
       </c>
       <c r="M34" t="n">
-        <v>367.183382776917</v>
+        <v>1240.13155872774</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0138217730801552</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0138312973780746</v>
+        <v>0.0113265843676149</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0138217730801552</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="Q34" t="s">
         <v>23</v>
@@ -12144,40 +12144,40 @@
         <v>50</v>
       </c>
       <c r="E35" t="n">
-        <v>20362</v>
+        <v>1583</v>
       </c>
       <c r="F35" t="n">
-        <v>20342</v>
+        <v>1583</v>
       </c>
       <c r="G35" t="n">
-        <v>20362</v>
+        <v>1583</v>
       </c>
       <c r="H35" t="n">
-        <v>0.806479721166033</v>
+        <v>0.0626980354879594</v>
       </c>
       <c r="I35" t="n">
-        <v>0.806326304106548</v>
+        <v>0.0627477406056762</v>
       </c>
       <c r="J35" t="n">
-        <v>0.806479721166033</v>
+        <v>0.0626980354879594</v>
       </c>
       <c r="K35" t="n">
-        <v>994.901181410119</v>
+        <v>367.183382776917</v>
       </c>
       <c r="L35" t="n">
-        <v>997.536938408173</v>
+        <v>367.183382776917</v>
       </c>
       <c r="M35" t="n">
-        <v>994.901181410119</v>
+        <v>367.183382776917</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0211425382318378</v>
+        <v>0.0138217730801552</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0211213458731485</v>
+        <v>0.0138312973780746</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0211425382318378</v>
+        <v>0.0138217730801552</v>
       </c>
       <c r="Q35" t="s">
         <v>23</v>
@@ -12206,40 +12206,40 @@
         <v>50</v>
       </c>
       <c r="E36" t="n">
-        <v>25248</v>
+        <v>20362</v>
       </c>
       <c r="F36" t="n">
-        <v>25228</v>
+        <v>20342</v>
       </c>
       <c r="G36" t="n">
-        <v>25248</v>
+        <v>20362</v>
       </c>
       <c r="H36" t="n">
-        <v>0.235381861575179</v>
+        <v>0.806479721166033</v>
       </c>
       <c r="I36" t="n">
-        <v>0.235239267464847</v>
+        <v>0.806326304106548</v>
       </c>
       <c r="J36" t="n">
-        <v>0.235381861575179</v>
+        <v>0.806479721166033</v>
       </c>
       <c r="K36" t="n">
-        <v>1240.13155872774</v>
+        <v>994.901181410119</v>
       </c>
       <c r="L36" t="n">
-        <v>1245.12493895292</v>
+        <v>997.536938408173</v>
       </c>
       <c r="M36" t="n">
-        <v>1240.13155872774</v>
+        <v>994.901181410119</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0211425382318378</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0113265843676149</v>
+        <v>0.0211213458731485</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0211425382318378</v>
       </c>
       <c r="Q36" t="s">
         <v>23</v>
@@ -12888,40 +12888,40 @@
         <v>50</v>
       </c>
       <c r="E47" t="n">
-        <v>5195</v>
+        <v>85103</v>
       </c>
       <c r="F47" t="n">
-        <v>5195</v>
+        <v>84980</v>
       </c>
       <c r="G47" t="n">
-        <v>5195</v>
+        <v>85103</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0610436764861403</v>
+        <v>0.245462280613201</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0611320310661332</v>
+        <v>0.245212187316949</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0610436764861403</v>
+        <v>0.245462280613201</v>
       </c>
       <c r="K47" t="n">
-        <v>800.575802373673</v>
+        <v>2232.66124375598</v>
       </c>
       <c r="L47" t="n">
-        <v>800.575802373673</v>
+        <v>2254.43880155406</v>
       </c>
       <c r="M47" t="n">
-        <v>800.575802373673</v>
+        <v>2232.66124375598</v>
       </c>
       <c r="N47" t="n">
-        <v>0.00950324665414531</v>
+        <v>0.00644852439127257</v>
       </c>
       <c r="O47" t="n">
-        <v>0.00952487560443041</v>
+        <v>0.00649010549686332</v>
       </c>
       <c r="P47" t="n">
-        <v>0.00950324665414531</v>
+        <v>0.00644852439127257</v>
       </c>
       <c r="Q47" t="s">
         <v>23</v>
@@ -12950,40 +12950,40 @@
         <v>50</v>
       </c>
       <c r="E48" t="n">
-        <v>60478</v>
+        <v>5195</v>
       </c>
       <c r="F48" t="n">
-        <v>60405</v>
+        <v>5195</v>
       </c>
       <c r="G48" t="n">
-        <v>60478</v>
+        <v>5195</v>
       </c>
       <c r="H48" t="n">
-        <v>0.710644748128738</v>
+        <v>0.0610436764861403</v>
       </c>
       <c r="I48" t="n">
-        <v>0.710814309249235</v>
+        <v>0.0611320310661332</v>
       </c>
       <c r="J48" t="n">
-        <v>0.710644748128738</v>
+        <v>0.0610436764861403</v>
       </c>
       <c r="K48" t="n">
-        <v>2114.73464289524</v>
+        <v>800.575802373673</v>
       </c>
       <c r="L48" t="n">
-        <v>2130.04494163151</v>
+        <v>800.575802373673</v>
       </c>
       <c r="M48" t="n">
-        <v>2114.73464289524</v>
+        <v>800.575802373673</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0153635742182986</v>
+        <v>0.00950324665414531</v>
       </c>
       <c r="O48" t="n">
-        <v>0.0154265494221258</v>
+        <v>0.00952487560443041</v>
       </c>
       <c r="P48" t="n">
-        <v>0.0153635742182986</v>
+        <v>0.00950324665414531</v>
       </c>
       <c r="Q48" t="s">
         <v>23</v>
@@ -13012,40 +13012,40 @@
         <v>50</v>
       </c>
       <c r="E49" t="n">
-        <v>85103</v>
+        <v>60478</v>
       </c>
       <c r="F49" t="n">
-        <v>84980</v>
+        <v>60405</v>
       </c>
       <c r="G49" t="n">
-        <v>85103</v>
+        <v>60478</v>
       </c>
       <c r="H49" t="n">
-        <v>0.245462280613201</v>
+        <v>0.710644748128738</v>
       </c>
       <c r="I49" t="n">
-        <v>0.245212187316949</v>
+        <v>0.710814309249235</v>
       </c>
       <c r="J49" t="n">
-        <v>0.245462280613201</v>
+        <v>0.710644748128738</v>
       </c>
       <c r="K49" t="n">
-        <v>2232.66124375598</v>
+        <v>2114.73464289524</v>
       </c>
       <c r="L49" t="n">
-        <v>2254.43880155406</v>
+        <v>2130.04494163151</v>
       </c>
       <c r="M49" t="n">
-        <v>2232.66124375598</v>
+        <v>2114.73464289524</v>
       </c>
       <c r="N49" t="n">
-        <v>0.00644852439127257</v>
+        <v>0.0153635742182986</v>
       </c>
       <c r="O49" t="n">
-        <v>0.00649010549686332</v>
+        <v>0.0154265494221258</v>
       </c>
       <c r="P49" t="n">
-        <v>0.00644852439127257</v>
+        <v>0.0153635742182986</v>
       </c>
       <c r="Q49" t="s">
         <v>23</v>
@@ -13694,40 +13694,40 @@
         <v>50</v>
       </c>
       <c r="E60" t="n">
-        <v>3409</v>
+        <v>72182</v>
       </c>
       <c r="F60" t="n">
-        <v>3409</v>
+        <v>72049</v>
       </c>
       <c r="G60" t="n">
-        <v>3409</v>
+        <v>72182</v>
       </c>
       <c r="H60" t="n">
-        <v>0.0472278407359175</v>
+        <v>0.231480917303505</v>
       </c>
       <c r="I60" t="n">
-        <v>0.0473150217213285</v>
+        <v>0.23115298979127</v>
       </c>
       <c r="J60" t="n">
-        <v>0.0472278407359175</v>
+        <v>0.231480917303505</v>
       </c>
       <c r="K60" t="n">
-        <v>592.233927153156</v>
+        <v>2455.15607980735</v>
       </c>
       <c r="L60" t="n">
-        <v>592.233927153156</v>
+        <v>2439.55895942381</v>
       </c>
       <c r="M60" t="n">
-        <v>592.233927153156</v>
+        <v>2455.15607980735</v>
       </c>
       <c r="N60" t="n">
-        <v>0.00820392037282418</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="O60" t="n">
-        <v>0.00821430188089977</v>
+        <v>0.00774704176324199</v>
       </c>
       <c r="P60" t="n">
-        <v>0.00820392037282418</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="Q60" t="s">
         <v>23</v>
@@ -13756,40 +13756,40 @@
         <v>50</v>
       </c>
       <c r="E61" t="n">
-        <v>56150</v>
+        <v>3409</v>
       </c>
       <c r="F61" t="n">
-        <v>56126</v>
+        <v>3409</v>
       </c>
       <c r="G61" t="n">
-        <v>56150</v>
+        <v>3409</v>
       </c>
       <c r="H61" t="n">
-        <v>0.777894766008146</v>
+        <v>0.0472278407359175</v>
       </c>
       <c r="I61" t="n">
-        <v>0.77899762661522</v>
+        <v>0.0473150217213285</v>
       </c>
       <c r="J61" t="n">
-        <v>0.777894766008146</v>
+        <v>0.0472278407359175</v>
       </c>
       <c r="K61" t="n">
-        <v>1998.48601915206</v>
+        <v>592.233927153156</v>
       </c>
       <c r="L61" t="n">
-        <v>2000.98194886161</v>
+        <v>592.233927153156</v>
       </c>
       <c r="M61" t="n">
-        <v>1998.48601915206</v>
+        <v>592.233927153156</v>
       </c>
       <c r="N61" t="n">
-        <v>0.0153151457594137</v>
+        <v>0.00820392037282418</v>
       </c>
       <c r="O61" t="n">
-        <v>0.0152087577905497</v>
+        <v>0.00821430188089977</v>
       </c>
       <c r="P61" t="n">
-        <v>0.0153151457594137</v>
+        <v>0.00820392037282418</v>
       </c>
       <c r="Q61" t="s">
         <v>23</v>
@@ -13818,40 +13818,40 @@
         <v>50</v>
       </c>
       <c r="E62" t="n">
-        <v>72182</v>
+        <v>56150</v>
       </c>
       <c r="F62" t="n">
-        <v>72049</v>
+        <v>56126</v>
       </c>
       <c r="G62" t="n">
-        <v>72182</v>
+        <v>56150</v>
       </c>
       <c r="H62" t="n">
-        <v>0.231480917303505</v>
+        <v>0.777894766008146</v>
       </c>
       <c r="I62" t="n">
-        <v>0.23115298979127</v>
+        <v>0.77899762661522</v>
       </c>
       <c r="J62" t="n">
-        <v>0.231480917303505</v>
+        <v>0.777894766008146</v>
       </c>
       <c r="K62" t="n">
-        <v>2455.15607980735</v>
+        <v>1998.48601915206</v>
       </c>
       <c r="L62" t="n">
-        <v>2439.55895942381</v>
+        <v>2000.98194886161</v>
       </c>
       <c r="M62" t="n">
-        <v>2455.15607980735</v>
+        <v>1998.48601915206</v>
       </c>
       <c r="N62" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.0153151457594137</v>
       </c>
       <c r="O62" t="n">
-        <v>0.00774704176324199</v>
+        <v>0.0152087577905497</v>
       </c>
       <c r="P62" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.0153151457594137</v>
       </c>
       <c r="Q62" t="s">
         <v>23</v>
@@ -14576,40 +14576,40 @@
         <v>50</v>
       </c>
       <c r="E8" t="n">
-        <v>65735</v>
+        <v>1225930</v>
       </c>
       <c r="F8" t="n">
-        <v>22627</v>
+        <v>1225803</v>
       </c>
       <c r="G8" t="n">
-        <v>20365</v>
+        <v>1225930</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0536205166689778</v>
+        <v>0.72385314979715</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0184589203974864</v>
+        <v>0.724066742983516</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0166118783291053</v>
+        <v>0.72385314979715</v>
       </c>
       <c r="K8" t="n">
-        <v>2474.29871298895</v>
+        <v>6292.05513549448</v>
       </c>
       <c r="L8" t="n">
-        <v>1662.96311816363</v>
+        <v>6298.22140556721</v>
       </c>
       <c r="M8" t="n">
-        <v>1455.59974768693</v>
+        <v>6292.05513549448</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00200596629495626</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="O8" t="n">
-        <v>0.00135780707407631</v>
+        <v>0.00327260898423871</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00119130073452516</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -14638,40 +14638,40 @@
         <v>50</v>
       </c>
       <c r="E9" t="n">
-        <v>793881</v>
+        <v>65735</v>
       </c>
       <c r="F9" t="n">
-        <v>655535</v>
+        <v>22627</v>
       </c>
       <c r="G9" t="n">
-        <v>636168</v>
+        <v>20365</v>
       </c>
       <c r="H9" t="n">
-        <v>0.647574494465426</v>
+        <v>0.0536205166689778</v>
       </c>
       <c r="I9" t="n">
-        <v>0.534780058459638</v>
+        <v>0.0184589203974864</v>
       </c>
       <c r="J9" t="n">
-        <v>0.518926855530087</v>
+        <v>0.0166118783291053</v>
       </c>
       <c r="K9" t="n">
-        <v>5814.84224063871</v>
+        <v>2474.29871298895</v>
       </c>
       <c r="L9" t="n">
-        <v>5060.82232845809</v>
+        <v>1662.96311816363</v>
       </c>
       <c r="M9" t="n">
-        <v>5119.44603051822</v>
+        <v>1455.59974768693</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00297386642019264</v>
+        <v>0.00200596629495626</v>
       </c>
       <c r="O9" t="n">
-        <v>0.00274427536456074</v>
+        <v>0.00135780707407631</v>
       </c>
       <c r="P9" t="n">
-        <v>0.00299876214304256</v>
+        <v>0.00119130073452516</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -14700,40 +14700,40 @@
         <v>50</v>
       </c>
       <c r="E10" t="n">
-        <v>1225930</v>
+        <v>793881</v>
       </c>
       <c r="F10" t="n">
-        <v>1225803</v>
+        <v>655535</v>
       </c>
       <c r="G10" t="n">
-        <v>1225930</v>
+        <v>636168</v>
       </c>
       <c r="H10" t="n">
-        <v>0.72385314979715</v>
+        <v>0.647574494465426</v>
       </c>
       <c r="I10" t="n">
-        <v>0.724066742983516</v>
+        <v>0.534780058459638</v>
       </c>
       <c r="J10" t="n">
-        <v>0.72385314979715</v>
+        <v>0.518926855530087</v>
       </c>
       <c r="K10" t="n">
-        <v>6292.05513549448</v>
+        <v>5814.84224063871</v>
       </c>
       <c r="L10" t="n">
-        <v>6298.22140556721</v>
+        <v>5060.82232845809</v>
       </c>
       <c r="M10" t="n">
-        <v>6292.05513549448</v>
+        <v>5119.44603051822</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00297386642019264</v>
       </c>
       <c r="O10" t="n">
-        <v>0.00327260898423871</v>
+        <v>0.00274427536456074</v>
       </c>
       <c r="P10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00299876214304256</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -15538,40 +15538,40 @@
         <v>50</v>
       </c>
       <c r="E24" t="n">
-        <v>31925</v>
+        <v>642667</v>
       </c>
       <c r="F24" t="n">
-        <v>10640</v>
+        <v>642565</v>
       </c>
       <c r="G24" t="n">
-        <v>9604</v>
+        <v>642667</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0496758041100601</v>
+        <v>0.692662701102907</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0165586360912904</v>
+        <v>0.692832043232659</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0149439756514649</v>
+        <v>0.692662701102907</v>
       </c>
       <c r="K24" t="n">
-        <v>1887.26567187525</v>
+        <v>4626.22104388858</v>
       </c>
       <c r="L24" t="n">
-        <v>1337.34554369841</v>
+        <v>4628.15173571346</v>
       </c>
       <c r="M24" t="n">
-        <v>1108.47980485663</v>
+        <v>4626.22104388858</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0029246552583609</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="O24" t="n">
-        <v>0.00206847613429708</v>
+        <v>0.00449309450544533</v>
       </c>
       <c r="P24" t="n">
-        <v>0.00171185706555702</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="Q24" t="s">
         <v>23</v>
@@ -15600,40 +15600,40 @@
         <v>50</v>
       </c>
       <c r="E25" t="n">
-        <v>383636</v>
+        <v>31925</v>
       </c>
       <c r="F25" t="n">
-        <v>311212</v>
+        <v>10640</v>
       </c>
       <c r="G25" t="n">
-        <v>304101</v>
+        <v>9604</v>
       </c>
       <c r="H25" t="n">
-        <v>0.596943673784402</v>
+        <v>0.0496758041100601</v>
       </c>
       <c r="I25" t="n">
-        <v>0.484327655567919</v>
+        <v>0.0165586360912904</v>
       </c>
       <c r="J25" t="n">
-        <v>0.473185957891101</v>
+        <v>0.0149439756514649</v>
       </c>
       <c r="K25" t="n">
-        <v>4095.13287589014</v>
+        <v>1887.26567187525</v>
       </c>
       <c r="L25" t="n">
-        <v>3369.53323132244</v>
+        <v>1337.34554369841</v>
       </c>
       <c r="M25" t="n">
-        <v>3472.84881243213</v>
+        <v>1108.47980485663</v>
       </c>
       <c r="N25" t="n">
-        <v>0.00430134638534656</v>
+        <v>0.0029246552583609</v>
       </c>
       <c r="O25" t="n">
-        <v>0.00366948826611233</v>
+        <v>0.00206847613429708</v>
       </c>
       <c r="P25" t="n">
-        <v>0.00394456144798949</v>
+        <v>0.00171185706555702</v>
       </c>
       <c r="Q25" t="s">
         <v>23</v>
@@ -15662,40 +15662,40 @@
         <v>50</v>
       </c>
       <c r="E26" t="n">
-        <v>642667</v>
+        <v>383636</v>
       </c>
       <c r="F26" t="n">
-        <v>642565</v>
+        <v>311212</v>
       </c>
       <c r="G26" t="n">
-        <v>642667</v>
+        <v>304101</v>
       </c>
       <c r="H26" t="n">
-        <v>0.692662701102907</v>
+        <v>0.596943673784402</v>
       </c>
       <c r="I26" t="n">
-        <v>0.692832043232659</v>
+        <v>0.484327655567919</v>
       </c>
       <c r="J26" t="n">
-        <v>0.692662701102907</v>
+        <v>0.473185957891101</v>
       </c>
       <c r="K26" t="n">
-        <v>4626.22104388858</v>
+        <v>4095.13287589014</v>
       </c>
       <c r="L26" t="n">
-        <v>4628.15173571346</v>
+        <v>3369.53323132244</v>
       </c>
       <c r="M26" t="n">
-        <v>4626.22104388858</v>
+        <v>3472.84881243213</v>
       </c>
       <c r="N26" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00430134638534656</v>
       </c>
       <c r="O26" t="n">
-        <v>0.00449309450544533</v>
+        <v>0.00366948826611233</v>
       </c>
       <c r="P26" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00394456144798949</v>
       </c>
       <c r="Q26" t="s">
         <v>23</v>
@@ -16500,40 +16500,40 @@
         <v>50</v>
       </c>
       <c r="E40" t="n">
-        <v>4170</v>
+        <v>82016</v>
       </c>
       <c r="F40" t="n">
-        <v>1523</v>
+        <v>82016</v>
       </c>
       <c r="G40" t="n">
-        <v>1384</v>
+        <v>82016</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0508437378072571</v>
+        <v>0.764618138424821</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0185695474053843</v>
+        <v>0.764760732535154</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0168747561451424</v>
+        <v>0.764618138424821</v>
       </c>
       <c r="K40" t="n">
-        <v>524.416092754599</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="L40" t="n">
-        <v>299.792844360902</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="M40" t="n">
-        <v>286.149865937851</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="N40" t="n">
-        <v>0.00633768612955597</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0036574132905182</v>
+        <v>0.0113265843676149</v>
       </c>
       <c r="P40" t="n">
-        <v>0.00347463222320292</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="Q40" t="s">
         <v>23</v>
@@ -16562,40 +16562,40 @@
         <v>50</v>
       </c>
       <c r="E41" t="n">
-        <v>64736</v>
+        <v>4170</v>
       </c>
       <c r="F41" t="n">
-        <v>54991</v>
+        <v>1523</v>
       </c>
       <c r="G41" t="n">
-        <v>53126</v>
+        <v>1384</v>
       </c>
       <c r="H41" t="n">
-        <v>0.789309403043309</v>
+        <v>0.0508437378072571</v>
       </c>
       <c r="I41" t="n">
-        <v>0.670491123683184</v>
+        <v>0.0185695474053843</v>
       </c>
       <c r="J41" t="n">
-        <v>0.647751658213032</v>
+        <v>0.0168747561451424</v>
       </c>
       <c r="K41" t="n">
-        <v>1210.94979765523</v>
+        <v>524.416092754599</v>
       </c>
       <c r="L41" t="n">
-        <v>1240.6277659818</v>
+        <v>299.792844360902</v>
       </c>
       <c r="M41" t="n">
-        <v>1208.74936924544</v>
+        <v>286.149865937851</v>
       </c>
       <c r="N41" t="n">
-        <v>0.00931194669267898</v>
+        <v>0.00633768612955597</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0113234610137819</v>
+        <v>0.0036574132905182</v>
       </c>
       <c r="P41" t="n">
-        <v>0.0112307730915826</v>
+        <v>0.00347463222320292</v>
       </c>
       <c r="Q41" t="s">
         <v>23</v>
@@ -16624,40 +16624,40 @@
         <v>50</v>
       </c>
       <c r="E42" t="n">
-        <v>82016</v>
+        <v>64736</v>
       </c>
       <c r="F42" t="n">
-        <v>82016</v>
+        <v>54991</v>
       </c>
       <c r="G42" t="n">
-        <v>82016</v>
+        <v>53126</v>
       </c>
       <c r="H42" t="n">
-        <v>0.764618138424821</v>
+        <v>0.789309403043309</v>
       </c>
       <c r="I42" t="n">
-        <v>0.764760732535154</v>
+        <v>0.670491123683184</v>
       </c>
       <c r="J42" t="n">
-        <v>0.764618138424821</v>
+        <v>0.647751658213032</v>
       </c>
       <c r="K42" t="n">
-        <v>1309.15839613519</v>
+        <v>1210.94979765523</v>
       </c>
       <c r="L42" t="n">
-        <v>1309.15839613519</v>
+        <v>1240.6277659818</v>
       </c>
       <c r="M42" t="n">
-        <v>1309.15839613519</v>
+        <v>1208.74936924544</v>
       </c>
       <c r="N42" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.00931194669267898</v>
       </c>
       <c r="O42" t="n">
-        <v>0.0113265843676149</v>
+        <v>0.0113234610137819</v>
       </c>
       <c r="P42" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0112307730915826</v>
       </c>
       <c r="Q42" t="s">
         <v>23</v>
@@ -17462,40 +17462,40 @@
         <v>50</v>
       </c>
       <c r="E56" t="n">
-        <v>18750</v>
+        <v>261602</v>
       </c>
       <c r="F56" t="n">
-        <v>6495</v>
+        <v>261577</v>
       </c>
       <c r="G56" t="n">
-        <v>5686</v>
+        <v>261602</v>
       </c>
       <c r="H56" t="n">
-        <v>0.0716737639620492</v>
+        <v>0.754537719386799</v>
       </c>
       <c r="I56" t="n">
-        <v>0.0248301647316087</v>
+        <v>0.754787812683051</v>
       </c>
       <c r="J56" t="n">
-        <v>0.021735307834038</v>
+        <v>0.754537719386799</v>
       </c>
       <c r="K56" t="n">
-        <v>1242.4073636488</v>
+        <v>2501.32257198692</v>
       </c>
       <c r="L56" t="n">
-        <v>809.74930757766</v>
+        <v>2500.28720132083</v>
       </c>
       <c r="M56" t="n">
-        <v>712.80851027292</v>
+        <v>2501.32257198692</v>
       </c>
       <c r="N56" t="n">
-        <v>0.00471669847814188</v>
+        <v>0.00644852439127255</v>
       </c>
       <c r="O56" t="n">
-        <v>0.00310336492896555</v>
+        <v>0.00649010549686331</v>
       </c>
       <c r="P56" t="n">
-        <v>0.0027395071922153</v>
+        <v>0.00644852439127255</v>
       </c>
       <c r="Q56" t="s">
         <v>23</v>
@@ -17524,40 +17524,40 @@
         <v>50</v>
       </c>
       <c r="E57" t="n">
-        <v>179301</v>
+        <v>18750</v>
       </c>
       <c r="F57" t="n">
-        <v>147690</v>
+        <v>6495</v>
       </c>
       <c r="G57" t="n">
-        <v>141989</v>
+        <v>5686</v>
       </c>
       <c r="H57" t="n">
-        <v>0.685396136115167</v>
+        <v>0.0716737639620492</v>
       </c>
       <c r="I57" t="n">
-        <v>0.564613861310436</v>
+        <v>0.0248301647316087</v>
       </c>
       <c r="J57" t="n">
-        <v>0.542767257131062</v>
+        <v>0.021735307834038</v>
       </c>
       <c r="K57" t="n">
-        <v>2122.68338987206</v>
+        <v>1242.4073636488</v>
       </c>
       <c r="L57" t="n">
-        <v>1811.25884655811</v>
+        <v>809.74930757766</v>
       </c>
       <c r="M57" t="n">
-        <v>1895.27634691521</v>
+        <v>712.80851027292</v>
       </c>
       <c r="N57" t="n">
-        <v>0.00612002931455315</v>
+        <v>0.00471669847814188</v>
       </c>
       <c r="O57" t="n">
-        <v>0.0053294207179917</v>
+        <v>0.00310336492896555</v>
       </c>
       <c r="P57" t="n">
-        <v>0.0061204535387096</v>
+        <v>0.0027395071922153</v>
       </c>
       <c r="Q57" t="s">
         <v>23</v>
@@ -17586,40 +17586,40 @@
         <v>50</v>
       </c>
       <c r="E58" t="n">
-        <v>261602</v>
+        <v>179301</v>
       </c>
       <c r="F58" t="n">
-        <v>261577</v>
+        <v>147690</v>
       </c>
       <c r="G58" t="n">
-        <v>261602</v>
+        <v>141989</v>
       </c>
       <c r="H58" t="n">
-        <v>0.754537719386799</v>
+        <v>0.685396136115167</v>
       </c>
       <c r="I58" t="n">
-        <v>0.754787812683051</v>
+        <v>0.564613861310436</v>
       </c>
       <c r="J58" t="n">
-        <v>0.754537719386799</v>
+        <v>0.542767257131062</v>
       </c>
       <c r="K58" t="n">
-        <v>2501.32257198692</v>
+        <v>2122.68338987206</v>
       </c>
       <c r="L58" t="n">
-        <v>2500.28720132083</v>
+        <v>1811.25884655811</v>
       </c>
       <c r="M58" t="n">
-        <v>2501.32257198692</v>
+        <v>1895.27634691521</v>
       </c>
       <c r="N58" t="n">
-        <v>0.00644852439127255</v>
+        <v>0.00612002931455315</v>
       </c>
       <c r="O58" t="n">
-        <v>0.00649010549686331</v>
+        <v>0.0053294207179917</v>
       </c>
       <c r="P58" t="n">
-        <v>0.00644852439127255</v>
+        <v>0.0061204535387096</v>
       </c>
       <c r="Q58" t="s">
         <v>23</v>
@@ -18424,40 +18424,40 @@
         <v>50</v>
       </c>
       <c r="E72" t="n">
-        <v>10890</v>
+        <v>239645</v>
       </c>
       <c r="F72" t="n">
-        <v>3969</v>
+        <v>239645</v>
       </c>
       <c r="G72" t="n">
-        <v>3691</v>
+        <v>239645</v>
       </c>
       <c r="H72" t="n">
-        <v>0.045442216612072</v>
+        <v>0.768519082696495</v>
       </c>
       <c r="I72" t="n">
-        <v>0.0165619979553089</v>
+        <v>0.76884701020873</v>
       </c>
       <c r="J72" t="n">
-        <v>0.0154019487158088</v>
+        <v>0.768519082696495</v>
       </c>
       <c r="K72" t="n">
-        <v>847.453087125624</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="L72" t="n">
-        <v>607.97428572679</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="M72" t="n">
-        <v>616.82608672745</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="N72" t="n">
-        <v>0.00356500723312259</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="O72" t="n">
-        <v>0.002539866097422</v>
+        <v>0.00774704176324198</v>
       </c>
       <c r="P72" t="n">
-        <v>0.00257712385489421</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="Q72" t="s">
         <v>23</v>
@@ -18486,40 +18486,40 @@
         <v>50</v>
       </c>
       <c r="E73" t="n">
-        <v>166208</v>
+        <v>10890</v>
       </c>
       <c r="F73" t="n">
-        <v>141642</v>
+        <v>3969</v>
       </c>
       <c r="G73" t="n">
-        <v>136952</v>
+        <v>3691</v>
       </c>
       <c r="H73" t="n">
-        <v>0.69355922301738</v>
+        <v>0.045442216612072</v>
       </c>
       <c r="I73" t="n">
-        <v>0.591049260364289</v>
+        <v>0.0165619979553089</v>
       </c>
       <c r="J73" t="n">
-        <v>0.571478645496464</v>
+        <v>0.0154019487158088</v>
       </c>
       <c r="K73" t="n">
-        <v>2287.87585247375</v>
+        <v>847.453087125624</v>
       </c>
       <c r="L73" t="n">
-        <v>2107.858318533</v>
+        <v>607.97428572679</v>
       </c>
       <c r="M73" t="n">
-        <v>1957.33924894932</v>
+        <v>616.82608672745</v>
       </c>
       <c r="N73" t="n">
-        <v>0.00607006523918823</v>
+        <v>0.00356500723312259</v>
       </c>
       <c r="O73" t="n">
-        <v>0.00539918277279873</v>
+        <v>0.002539866097422</v>
       </c>
       <c r="P73" t="n">
-        <v>0.00555214543106352</v>
+        <v>0.00257712385489421</v>
       </c>
       <c r="Q73" t="s">
         <v>23</v>
@@ -18548,40 +18548,40 @@
         <v>50</v>
       </c>
       <c r="E74" t="n">
-        <v>239645</v>
+        <v>166208</v>
       </c>
       <c r="F74" t="n">
-        <v>239645</v>
+        <v>141642</v>
       </c>
       <c r="G74" t="n">
-        <v>239645</v>
+        <v>136952</v>
       </c>
       <c r="H74" t="n">
-        <v>0.768519082696495</v>
+        <v>0.69355922301738</v>
       </c>
       <c r="I74" t="n">
-        <v>0.76884701020873</v>
+        <v>0.591049260364289</v>
       </c>
       <c r="J74" t="n">
-        <v>0.768519082696495</v>
+        <v>0.571478645496464</v>
       </c>
       <c r="K74" t="n">
-        <v>2556.52132729956</v>
+        <v>2287.87585247375</v>
       </c>
       <c r="L74" t="n">
-        <v>2556.52132729956</v>
+        <v>2107.858318533</v>
       </c>
       <c r="M74" t="n">
-        <v>2556.52132729956</v>
+        <v>1957.33924894932</v>
       </c>
       <c r="N74" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.00607006523918823</v>
       </c>
       <c r="O74" t="n">
-        <v>0.00774704176324198</v>
+        <v>0.00539918277279873</v>
       </c>
       <c r="P74" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.00555214543106352</v>
       </c>
       <c r="Q74" t="s">
         <v>23</v>
@@ -19462,40 +19462,40 @@
         <v>52</v>
       </c>
       <c r="E8" t="n">
-        <v>27739</v>
+        <v>467687</v>
       </c>
       <c r="F8" t="n">
-        <v>27739</v>
+        <v>467139</v>
       </c>
       <c r="G8" t="n">
-        <v>27739</v>
+        <v>467687</v>
       </c>
       <c r="H8" t="n">
-        <v>0.059311034944311</v>
+        <v>0.27614685020285</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0593806126227954</v>
+        <v>0.275933257016484</v>
       </c>
       <c r="J8" t="n">
-        <v>0.059311034944311</v>
+        <v>0.27614685020285</v>
       </c>
       <c r="K8" t="n">
-        <v>1753.3935316929</v>
+        <v>5531.81571257474</v>
       </c>
       <c r="L8" t="n">
-        <v>1753.3935316929</v>
+        <v>5549.62373270736</v>
       </c>
       <c r="M8" t="n">
-        <v>1753.3935316929</v>
+        <v>5531.81571257474</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00371504389479169</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="O8" t="n">
-        <v>0.00372398890528343</v>
+        <v>0.00327260898423871</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00371504389479169</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -19524,40 +19524,40 @@
         <v>52</v>
       </c>
       <c r="E9" t="n">
-        <v>316868</v>
+        <v>27739</v>
       </c>
       <c r="F9" t="n">
-        <v>316527</v>
+        <v>27739</v>
       </c>
       <c r="G9" t="n">
-        <v>316868</v>
+        <v>27739</v>
       </c>
       <c r="H9" t="n">
-        <v>0.677521504767077</v>
+        <v>0.059311034944311</v>
       </c>
       <c r="I9" t="n">
-        <v>0.677586328694457</v>
+        <v>0.0593806126227954</v>
       </c>
       <c r="J9" t="n">
-        <v>0.677521504767077</v>
+        <v>0.059311034944311</v>
       </c>
       <c r="K9" t="n">
-        <v>5104.49905281275</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="L9" t="n">
-        <v>5134.47976547479</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="M9" t="n">
-        <v>5104.49905281275</v>
+        <v>1753.3935316929</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00640203655040979</v>
+        <v>0.00371504389479169</v>
       </c>
       <c r="O9" t="n">
-        <v>0.00641730044991988</v>
+        <v>0.00372398890528343</v>
       </c>
       <c r="P9" t="n">
-        <v>0.00640203655040979</v>
+        <v>0.00371504389479169</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -19586,40 +19586,40 @@
         <v>52</v>
       </c>
       <c r="E10" t="n">
-        <v>467687</v>
+        <v>316868</v>
       </c>
       <c r="F10" t="n">
-        <v>467139</v>
+        <v>316527</v>
       </c>
       <c r="G10" t="n">
-        <v>467687</v>
+        <v>316868</v>
       </c>
       <c r="H10" t="n">
-        <v>0.27614685020285</v>
+        <v>0.677521504767077</v>
       </c>
       <c r="I10" t="n">
-        <v>0.275933257016484</v>
+        <v>0.677586328694457</v>
       </c>
       <c r="J10" t="n">
-        <v>0.27614685020285</v>
+        <v>0.677521504767077</v>
       </c>
       <c r="K10" t="n">
-        <v>5531.81571257474</v>
+        <v>5104.49905281275</v>
       </c>
       <c r="L10" t="n">
-        <v>5549.62373270736</v>
+        <v>5134.47976547479</v>
       </c>
       <c r="M10" t="n">
-        <v>5531.81571257474</v>
+        <v>5104.49905281275</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00640203655040979</v>
       </c>
       <c r="O10" t="n">
-        <v>0.00327260898423871</v>
+        <v>0.00641730044991988</v>
       </c>
       <c r="P10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00640203655040979</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -20268,40 +20268,40 @@
         <v>52</v>
       </c>
       <c r="E21" t="n">
-        <v>17552</v>
+        <v>285154</v>
       </c>
       <c r="F21" t="n">
-        <v>17552</v>
+        <v>284882</v>
       </c>
       <c r="G21" t="n">
-        <v>17552</v>
+        <v>285154</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0615527048542191</v>
+        <v>0.307337298897093</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0616114742244157</v>
+        <v>0.307167956767341</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0615527048542191</v>
+        <v>0.307337298897093</v>
       </c>
       <c r="K21" t="n">
-        <v>1504.21367142354</v>
+        <v>4209.61907351589</v>
       </c>
       <c r="L21" t="n">
-        <v>1504.21367142354</v>
+        <v>4187.19517882451</v>
       </c>
       <c r="M21" t="n">
-        <v>1504.21367142354</v>
+        <v>4209.61907351589</v>
       </c>
       <c r="N21" t="n">
-        <v>0.00509752408308916</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="O21" t="n">
-        <v>0.00510862319866652</v>
+        <v>0.00449309450544535</v>
       </c>
       <c r="P21" t="n">
-        <v>0.00509752408308916</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="Q21" t="s">
         <v>23</v>
@@ -20330,40 +20330,40 @@
         <v>52</v>
       </c>
       <c r="E22" t="n">
-        <v>179878</v>
+        <v>17552</v>
       </c>
       <c r="F22" t="n">
-        <v>179654</v>
+        <v>17552</v>
       </c>
       <c r="G22" t="n">
-        <v>179878</v>
+        <v>17552</v>
       </c>
       <c r="H22" t="n">
-        <v>0.630810018446173</v>
+        <v>0.0615527048542191</v>
       </c>
       <c r="I22" t="n">
-        <v>0.630626013577551</v>
+        <v>0.0616114742244157</v>
       </c>
       <c r="J22" t="n">
-        <v>0.630810018446173</v>
+        <v>0.0615527048542191</v>
       </c>
       <c r="K22" t="n">
-        <v>3699.62021384155</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="L22" t="n">
-        <v>3711.27598370106</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="M22" t="n">
-        <v>3699.62021384155</v>
+        <v>1504.21367142354</v>
       </c>
       <c r="N22" t="n">
-        <v>0.00832008151040211</v>
+        <v>0.00509752408308916</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0083894374722481</v>
+        <v>0.00510862319866652</v>
       </c>
       <c r="P22" t="n">
-        <v>0.00832008151040211</v>
+        <v>0.00509752408308916</v>
       </c>
       <c r="Q22" t="s">
         <v>23</v>
@@ -20392,40 +20392,40 @@
         <v>52</v>
       </c>
       <c r="E23" t="n">
-        <v>285154</v>
+        <v>179878</v>
       </c>
       <c r="F23" t="n">
-        <v>284882</v>
+        <v>179654</v>
       </c>
       <c r="G23" t="n">
-        <v>285154</v>
+        <v>179878</v>
       </c>
       <c r="H23" t="n">
-        <v>0.307337298897093</v>
+        <v>0.630810018446173</v>
       </c>
       <c r="I23" t="n">
-        <v>0.307167956767341</v>
+        <v>0.630626013577551</v>
       </c>
       <c r="J23" t="n">
-        <v>0.307337298897093</v>
+        <v>0.630810018446173</v>
       </c>
       <c r="K23" t="n">
-        <v>4209.61907351589</v>
+        <v>3699.62021384155</v>
       </c>
       <c r="L23" t="n">
-        <v>4187.19517882451</v>
+        <v>3711.27598370106</v>
       </c>
       <c r="M23" t="n">
-        <v>4209.61907351589</v>
+        <v>3699.62021384155</v>
       </c>
       <c r="N23" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00832008151040211</v>
       </c>
       <c r="O23" t="n">
-        <v>0.00449309450544535</v>
+        <v>0.0083894374722481</v>
       </c>
       <c r="P23" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00832008151040211</v>
       </c>
       <c r="Q23" t="s">
         <v>23</v>
@@ -21074,40 +21074,40 @@
         <v>52</v>
       </c>
       <c r="E34" t="n">
-        <v>1583</v>
+        <v>25248</v>
       </c>
       <c r="F34" t="n">
-        <v>1583</v>
+        <v>25228</v>
       </c>
       <c r="G34" t="n">
-        <v>1583</v>
+        <v>25248</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0626980354879594</v>
+        <v>0.235381861575179</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0627477406056762</v>
+        <v>0.235239267464847</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0626980354879594</v>
+        <v>0.235381861575179</v>
       </c>
       <c r="K34" t="n">
-        <v>367.183382776917</v>
+        <v>1240.13155872774</v>
       </c>
       <c r="L34" t="n">
-        <v>367.183382776917</v>
+        <v>1245.12493895292</v>
       </c>
       <c r="M34" t="n">
-        <v>367.183382776917</v>
+        <v>1240.13155872774</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0138217730801552</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0138312973780746</v>
+        <v>0.0113265843676149</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0138217730801552</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="Q34" t="s">
         <v>23</v>
@@ -21136,40 +21136,40 @@
         <v>52</v>
       </c>
       <c r="E35" t="n">
-        <v>20362</v>
+        <v>1583</v>
       </c>
       <c r="F35" t="n">
-        <v>20342</v>
+        <v>1583</v>
       </c>
       <c r="G35" t="n">
-        <v>20362</v>
+        <v>1583</v>
       </c>
       <c r="H35" t="n">
-        <v>0.806479721166033</v>
+        <v>0.0626980354879594</v>
       </c>
       <c r="I35" t="n">
-        <v>0.806326304106548</v>
+        <v>0.0627477406056762</v>
       </c>
       <c r="J35" t="n">
-        <v>0.806479721166033</v>
+        <v>0.0626980354879594</v>
       </c>
       <c r="K35" t="n">
-        <v>994.901181410119</v>
+        <v>367.183382776917</v>
       </c>
       <c r="L35" t="n">
-        <v>997.536938408173</v>
+        <v>367.183382776917</v>
       </c>
       <c r="M35" t="n">
-        <v>994.901181410119</v>
+        <v>367.183382776917</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0211425382318378</v>
+        <v>0.0138217730801552</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0211213458731485</v>
+        <v>0.0138312973780746</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0211425382318378</v>
+        <v>0.0138217730801552</v>
       </c>
       <c r="Q35" t="s">
         <v>23</v>
@@ -21198,40 +21198,40 @@
         <v>52</v>
       </c>
       <c r="E36" t="n">
-        <v>25248</v>
+        <v>20362</v>
       </c>
       <c r="F36" t="n">
-        <v>25228</v>
+        <v>20342</v>
       </c>
       <c r="G36" t="n">
-        <v>25248</v>
+        <v>20362</v>
       </c>
       <c r="H36" t="n">
-        <v>0.235381861575179</v>
+        <v>0.806479721166033</v>
       </c>
       <c r="I36" t="n">
-        <v>0.235239267464847</v>
+        <v>0.806326304106548</v>
       </c>
       <c r="J36" t="n">
-        <v>0.235381861575179</v>
+        <v>0.806479721166033</v>
       </c>
       <c r="K36" t="n">
-        <v>1240.13155872774</v>
+        <v>994.901181410119</v>
       </c>
       <c r="L36" t="n">
-        <v>1245.12493895292</v>
+        <v>997.536938408173</v>
       </c>
       <c r="M36" t="n">
-        <v>1240.13155872774</v>
+        <v>994.901181410119</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0211425382318378</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0113265843676149</v>
+        <v>0.0211213458731485</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0211425382318378</v>
       </c>
       <c r="Q36" t="s">
         <v>23</v>
@@ -21880,40 +21880,40 @@
         <v>52</v>
       </c>
       <c r="E47" t="n">
-        <v>5195</v>
+        <v>85103</v>
       </c>
       <c r="F47" t="n">
-        <v>5195</v>
+        <v>84980</v>
       </c>
       <c r="G47" t="n">
-        <v>5195</v>
+        <v>85103</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0610436764861403</v>
+        <v>0.245462280613201</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0611320310661332</v>
+        <v>0.245212187316949</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0610436764861403</v>
+        <v>0.245462280613201</v>
       </c>
       <c r="K47" t="n">
-        <v>800.575802373673</v>
+        <v>2232.66124375598</v>
       </c>
       <c r="L47" t="n">
-        <v>800.575802373673</v>
+        <v>2254.43880155406</v>
       </c>
       <c r="M47" t="n">
-        <v>800.575802373673</v>
+        <v>2232.66124375598</v>
       </c>
       <c r="N47" t="n">
-        <v>0.00950324665414531</v>
+        <v>0.00644852439127257</v>
       </c>
       <c r="O47" t="n">
-        <v>0.00952487560443041</v>
+        <v>0.00649010549686332</v>
       </c>
       <c r="P47" t="n">
-        <v>0.00950324665414531</v>
+        <v>0.00644852439127257</v>
       </c>
       <c r="Q47" t="s">
         <v>23</v>
@@ -21942,40 +21942,40 @@
         <v>52</v>
       </c>
       <c r="E48" t="n">
-        <v>60478</v>
+        <v>5195</v>
       </c>
       <c r="F48" t="n">
-        <v>60405</v>
+        <v>5195</v>
       </c>
       <c r="G48" t="n">
-        <v>60478</v>
+        <v>5195</v>
       </c>
       <c r="H48" t="n">
-        <v>0.710644748128738</v>
+        <v>0.0610436764861403</v>
       </c>
       <c r="I48" t="n">
-        <v>0.710814309249235</v>
+        <v>0.0611320310661332</v>
       </c>
       <c r="J48" t="n">
-        <v>0.710644748128738</v>
+        <v>0.0610436764861403</v>
       </c>
       <c r="K48" t="n">
-        <v>2114.73464289524</v>
+        <v>800.575802373673</v>
       </c>
       <c r="L48" t="n">
-        <v>2130.04494163151</v>
+        <v>800.575802373673</v>
       </c>
       <c r="M48" t="n">
-        <v>2114.73464289524</v>
+        <v>800.575802373673</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0153635742182986</v>
+        <v>0.00950324665414531</v>
       </c>
       <c r="O48" t="n">
-        <v>0.0154265494221258</v>
+        <v>0.00952487560443041</v>
       </c>
       <c r="P48" t="n">
-        <v>0.0153635742182986</v>
+        <v>0.00950324665414531</v>
       </c>
       <c r="Q48" t="s">
         <v>23</v>
@@ -22004,40 +22004,40 @@
         <v>52</v>
       </c>
       <c r="E49" t="n">
-        <v>85103</v>
+        <v>60478</v>
       </c>
       <c r="F49" t="n">
-        <v>84980</v>
+        <v>60405</v>
       </c>
       <c r="G49" t="n">
-        <v>85103</v>
+        <v>60478</v>
       </c>
       <c r="H49" t="n">
-        <v>0.245462280613201</v>
+        <v>0.710644748128738</v>
       </c>
       <c r="I49" t="n">
-        <v>0.245212187316949</v>
+        <v>0.710814309249235</v>
       </c>
       <c r="J49" t="n">
-        <v>0.245462280613201</v>
+        <v>0.710644748128738</v>
       </c>
       <c r="K49" t="n">
-        <v>2232.66124375598</v>
+        <v>2114.73464289524</v>
       </c>
       <c r="L49" t="n">
-        <v>2254.43880155406</v>
+        <v>2130.04494163151</v>
       </c>
       <c r="M49" t="n">
-        <v>2232.66124375598</v>
+        <v>2114.73464289524</v>
       </c>
       <c r="N49" t="n">
-        <v>0.00644852439127257</v>
+        <v>0.0153635742182986</v>
       </c>
       <c r="O49" t="n">
-        <v>0.00649010549686332</v>
+        <v>0.0154265494221258</v>
       </c>
       <c r="P49" t="n">
-        <v>0.00644852439127257</v>
+        <v>0.0153635742182986</v>
       </c>
       <c r="Q49" t="s">
         <v>23</v>
@@ -22686,40 +22686,40 @@
         <v>52</v>
       </c>
       <c r="E60" t="n">
-        <v>3409</v>
+        <v>72182</v>
       </c>
       <c r="F60" t="n">
-        <v>3409</v>
+        <v>72049</v>
       </c>
       <c r="G60" t="n">
-        <v>3409</v>
+        <v>72182</v>
       </c>
       <c r="H60" t="n">
-        <v>0.0472278407359175</v>
+        <v>0.231480917303505</v>
       </c>
       <c r="I60" t="n">
-        <v>0.0473150217213285</v>
+        <v>0.23115298979127</v>
       </c>
       <c r="J60" t="n">
-        <v>0.0472278407359175</v>
+        <v>0.231480917303505</v>
       </c>
       <c r="K60" t="n">
-        <v>592.233927153156</v>
+        <v>2455.15607980735</v>
       </c>
       <c r="L60" t="n">
-        <v>592.233927153156</v>
+        <v>2439.55895942381</v>
       </c>
       <c r="M60" t="n">
-        <v>592.233927153156</v>
+        <v>2455.15607980735</v>
       </c>
       <c r="N60" t="n">
-        <v>0.00820392037282418</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="O60" t="n">
-        <v>0.00821430188089977</v>
+        <v>0.00774704176324199</v>
       </c>
       <c r="P60" t="n">
-        <v>0.00820392037282418</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="Q60" t="s">
         <v>23</v>
@@ -22748,40 +22748,40 @@
         <v>52</v>
       </c>
       <c r="E61" t="n">
-        <v>56150</v>
+        <v>3409</v>
       </c>
       <c r="F61" t="n">
-        <v>56126</v>
+        <v>3409</v>
       </c>
       <c r="G61" t="n">
-        <v>56150</v>
+        <v>3409</v>
       </c>
       <c r="H61" t="n">
-        <v>0.777894766008146</v>
+        <v>0.0472278407359175</v>
       </c>
       <c r="I61" t="n">
-        <v>0.77899762661522</v>
+        <v>0.0473150217213285</v>
       </c>
       <c r="J61" t="n">
-        <v>0.777894766008146</v>
+        <v>0.0472278407359175</v>
       </c>
       <c r="K61" t="n">
-        <v>1998.48601915206</v>
+        <v>592.233927153156</v>
       </c>
       <c r="L61" t="n">
-        <v>2000.98194886161</v>
+        <v>592.233927153156</v>
       </c>
       <c r="M61" t="n">
-        <v>1998.48601915206</v>
+        <v>592.233927153156</v>
       </c>
       <c r="N61" t="n">
-        <v>0.0153151457594137</v>
+        <v>0.00820392037282418</v>
       </c>
       <c r="O61" t="n">
-        <v>0.0152087577905497</v>
+        <v>0.00821430188089977</v>
       </c>
       <c r="P61" t="n">
-        <v>0.0153151457594137</v>
+        <v>0.00820392037282418</v>
       </c>
       <c r="Q61" t="s">
         <v>23</v>
@@ -22810,40 +22810,40 @@
         <v>52</v>
       </c>
       <c r="E62" t="n">
-        <v>72182</v>
+        <v>56150</v>
       </c>
       <c r="F62" t="n">
-        <v>72049</v>
+        <v>56126</v>
       </c>
       <c r="G62" t="n">
-        <v>72182</v>
+        <v>56150</v>
       </c>
       <c r="H62" t="n">
-        <v>0.231480917303505</v>
+        <v>0.777894766008146</v>
       </c>
       <c r="I62" t="n">
-        <v>0.23115298979127</v>
+        <v>0.77899762661522</v>
       </c>
       <c r="J62" t="n">
-        <v>0.231480917303505</v>
+        <v>0.777894766008146</v>
       </c>
       <c r="K62" t="n">
-        <v>2455.15607980735</v>
+        <v>1998.48601915206</v>
       </c>
       <c r="L62" t="n">
-        <v>2439.55895942381</v>
+        <v>2000.98194886161</v>
       </c>
       <c r="M62" t="n">
-        <v>2455.15607980735</v>
+        <v>1998.48601915206</v>
       </c>
       <c r="N62" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.0153151457594137</v>
       </c>
       <c r="O62" t="n">
-        <v>0.00774704176324199</v>
+        <v>0.0152087577905497</v>
       </c>
       <c r="P62" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.0153151457594137</v>
       </c>
       <c r="Q62" t="s">
         <v>23</v>
@@ -23568,40 +23568,40 @@
         <v>52</v>
       </c>
       <c r="E8" t="n">
-        <v>65735</v>
+        <v>1225930</v>
       </c>
       <c r="F8" t="n">
-        <v>22627</v>
+        <v>1225803</v>
       </c>
       <c r="G8" t="n">
-        <v>20365</v>
+        <v>1225930</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0536205166689778</v>
+        <v>0.72385314979715</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0184589203974864</v>
+        <v>0.724066742983516</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0166118783291053</v>
+        <v>0.72385314979715</v>
       </c>
       <c r="K8" t="n">
-        <v>2474.29871298895</v>
+        <v>6292.05513549448</v>
       </c>
       <c r="L8" t="n">
-        <v>1662.96311816363</v>
+        <v>6298.22140556721</v>
       </c>
       <c r="M8" t="n">
-        <v>1455.59974768693</v>
+        <v>6292.05513549448</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00200596629495626</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="O8" t="n">
-        <v>0.00135780707407631</v>
+        <v>0.00327260898423871</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00119130073452516</v>
+        <v>0.00326171985831935</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -23630,40 +23630,40 @@
         <v>52</v>
       </c>
       <c r="E9" t="n">
-        <v>793881</v>
+        <v>65735</v>
       </c>
       <c r="F9" t="n">
-        <v>655535</v>
+        <v>22627</v>
       </c>
       <c r="G9" t="n">
-        <v>636168</v>
+        <v>20365</v>
       </c>
       <c r="H9" t="n">
-        <v>0.647574494465426</v>
+        <v>0.0536205166689778</v>
       </c>
       <c r="I9" t="n">
-        <v>0.534780058459638</v>
+        <v>0.0184589203974864</v>
       </c>
       <c r="J9" t="n">
-        <v>0.518926855530087</v>
+        <v>0.0166118783291053</v>
       </c>
       <c r="K9" t="n">
-        <v>5814.84224063871</v>
+        <v>2474.29871298895</v>
       </c>
       <c r="L9" t="n">
-        <v>5060.82232845809</v>
+        <v>1662.96311816363</v>
       </c>
       <c r="M9" t="n">
-        <v>5119.44603051822</v>
+        <v>1455.59974768693</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00297386642019264</v>
+        <v>0.00200596629495626</v>
       </c>
       <c r="O9" t="n">
-        <v>0.00274427536456074</v>
+        <v>0.00135780707407631</v>
       </c>
       <c r="P9" t="n">
-        <v>0.00299876214304256</v>
+        <v>0.00119130073452516</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -23692,40 +23692,40 @@
         <v>52</v>
       </c>
       <c r="E10" t="n">
-        <v>1225930</v>
+        <v>793881</v>
       </c>
       <c r="F10" t="n">
-        <v>1225803</v>
+        <v>655535</v>
       </c>
       <c r="G10" t="n">
-        <v>1225930</v>
+        <v>636168</v>
       </c>
       <c r="H10" t="n">
-        <v>0.72385314979715</v>
+        <v>0.647574494465426</v>
       </c>
       <c r="I10" t="n">
-        <v>0.724066742983516</v>
+        <v>0.534780058459638</v>
       </c>
       <c r="J10" t="n">
-        <v>0.72385314979715</v>
+        <v>0.518926855530087</v>
       </c>
       <c r="K10" t="n">
-        <v>6292.05513549448</v>
+        <v>5814.84224063871</v>
       </c>
       <c r="L10" t="n">
-        <v>6298.22140556721</v>
+        <v>5060.82232845809</v>
       </c>
       <c r="M10" t="n">
-        <v>6292.05513549448</v>
+        <v>5119.44603051822</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00297386642019264</v>
       </c>
       <c r="O10" t="n">
-        <v>0.00327260898423871</v>
+        <v>0.00274427536456074</v>
       </c>
       <c r="P10" t="n">
-        <v>0.00326171985831935</v>
+        <v>0.00299876214304256</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -24478,40 +24478,40 @@
         <v>52</v>
       </c>
       <c r="E23" t="n">
-        <v>31925</v>
+        <v>642667</v>
       </c>
       <c r="F23" t="n">
-        <v>10640</v>
+        <v>642565</v>
       </c>
       <c r="G23" t="n">
-        <v>9604</v>
+        <v>642667</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0496758041100601</v>
+        <v>0.692662701102907</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0165586360912904</v>
+        <v>0.692832043232659</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0149439756514649</v>
+        <v>0.692662701102907</v>
       </c>
       <c r="K23" t="n">
-        <v>1887.26567187525</v>
+        <v>4626.22104388858</v>
       </c>
       <c r="L23" t="n">
-        <v>1337.34554369841</v>
+        <v>4628.15173571346</v>
       </c>
       <c r="M23" t="n">
-        <v>1108.47980485663</v>
+        <v>4626.22104388858</v>
       </c>
       <c r="N23" t="n">
-        <v>0.0029246552583609</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="O23" t="n">
-        <v>0.00206847613429708</v>
+        <v>0.00449309450544533</v>
       </c>
       <c r="P23" t="n">
-        <v>0.00171185706555702</v>
+        <v>0.00450258153459727</v>
       </c>
       <c r="Q23" t="s">
         <v>23</v>
@@ -24540,40 +24540,40 @@
         <v>52</v>
       </c>
       <c r="E24" t="n">
-        <v>383636</v>
+        <v>31925</v>
       </c>
       <c r="F24" t="n">
-        <v>311212</v>
+        <v>10640</v>
       </c>
       <c r="G24" t="n">
-        <v>304101</v>
+        <v>9604</v>
       </c>
       <c r="H24" t="n">
-        <v>0.596943673784402</v>
+        <v>0.0496758041100601</v>
       </c>
       <c r="I24" t="n">
-        <v>0.484327655567919</v>
+        <v>0.0165586360912904</v>
       </c>
       <c r="J24" t="n">
-        <v>0.473185957891101</v>
+        <v>0.0149439756514649</v>
       </c>
       <c r="K24" t="n">
-        <v>4095.13287589014</v>
+        <v>1887.26567187525</v>
       </c>
       <c r="L24" t="n">
-        <v>3369.53323132244</v>
+        <v>1337.34554369841</v>
       </c>
       <c r="M24" t="n">
-        <v>3472.84881243213</v>
+        <v>1108.47980485663</v>
       </c>
       <c r="N24" t="n">
-        <v>0.00430134638534656</v>
+        <v>0.0029246552583609</v>
       </c>
       <c r="O24" t="n">
-        <v>0.00366948826611233</v>
+        <v>0.00206847613429708</v>
       </c>
       <c r="P24" t="n">
-        <v>0.00394456144798949</v>
+        <v>0.00171185706555702</v>
       </c>
       <c r="Q24" t="s">
         <v>23</v>
@@ -24602,40 +24602,40 @@
         <v>52</v>
       </c>
       <c r="E25" t="n">
-        <v>642667</v>
+        <v>383636</v>
       </c>
       <c r="F25" t="n">
-        <v>642565</v>
+        <v>311212</v>
       </c>
       <c r="G25" t="n">
-        <v>642667</v>
+        <v>304101</v>
       </c>
       <c r="H25" t="n">
-        <v>0.692662701102907</v>
+        <v>0.596943673784402</v>
       </c>
       <c r="I25" t="n">
-        <v>0.692832043232659</v>
+        <v>0.484327655567919</v>
       </c>
       <c r="J25" t="n">
-        <v>0.692662701102907</v>
+        <v>0.473185957891101</v>
       </c>
       <c r="K25" t="n">
-        <v>4626.22104388858</v>
+        <v>4095.13287589014</v>
       </c>
       <c r="L25" t="n">
-        <v>4628.15173571346</v>
+        <v>3369.53323132244</v>
       </c>
       <c r="M25" t="n">
-        <v>4626.22104388858</v>
+        <v>3472.84881243213</v>
       </c>
       <c r="N25" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00430134638534656</v>
       </c>
       <c r="O25" t="n">
-        <v>0.00449309450544533</v>
+        <v>0.00366948826611233</v>
       </c>
       <c r="P25" t="n">
-        <v>0.00450258153459727</v>
+        <v>0.00394456144798949</v>
       </c>
       <c r="Q25" t="s">
         <v>23</v>
@@ -25388,40 +25388,40 @@
         <v>52</v>
       </c>
       <c r="E38" t="n">
-        <v>4170</v>
+        <v>82016</v>
       </c>
       <c r="F38" t="n">
-        <v>1523</v>
+        <v>82016</v>
       </c>
       <c r="G38" t="n">
-        <v>1384</v>
+        <v>82016</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0508437378072571</v>
+        <v>0.764618138424821</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0185695474053843</v>
+        <v>0.764760732535154</v>
       </c>
       <c r="J38" t="n">
-        <v>0.0168747561451424</v>
+        <v>0.764618138424821</v>
       </c>
       <c r="K38" t="n">
-        <v>524.416092754599</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="L38" t="n">
-        <v>299.792844360902</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="M38" t="n">
-        <v>286.149865937851</v>
+        <v>1309.15839613519</v>
       </c>
       <c r="N38" t="n">
-        <v>0.00633768612955597</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="O38" t="n">
-        <v>0.0036574132905182</v>
+        <v>0.0113265843676149</v>
       </c>
       <c r="P38" t="n">
-        <v>0.00347463222320292</v>
+        <v>0.0112906000951926</v>
       </c>
       <c r="Q38" t="s">
         <v>23</v>
@@ -25450,40 +25450,40 @@
         <v>52</v>
       </c>
       <c r="E39" t="n">
-        <v>64736</v>
+        <v>4170</v>
       </c>
       <c r="F39" t="n">
-        <v>54991</v>
+        <v>1523</v>
       </c>
       <c r="G39" t="n">
-        <v>53126</v>
+        <v>1384</v>
       </c>
       <c r="H39" t="n">
-        <v>0.789309403043309</v>
+        <v>0.0508437378072571</v>
       </c>
       <c r="I39" t="n">
-        <v>0.670491123683184</v>
+        <v>0.0185695474053843</v>
       </c>
       <c r="J39" t="n">
-        <v>0.647751658213032</v>
+        <v>0.0168747561451424</v>
       </c>
       <c r="K39" t="n">
-        <v>1210.94979765523</v>
+        <v>524.416092754599</v>
       </c>
       <c r="L39" t="n">
-        <v>1240.6277659818</v>
+        <v>299.792844360902</v>
       </c>
       <c r="M39" t="n">
-        <v>1208.74936924544</v>
+        <v>286.149865937851</v>
       </c>
       <c r="N39" t="n">
-        <v>0.00931194669267898</v>
+        <v>0.00633768612955597</v>
       </c>
       <c r="O39" t="n">
-        <v>0.0113234610137819</v>
+        <v>0.0036574132905182</v>
       </c>
       <c r="P39" t="n">
-        <v>0.0112307730915826</v>
+        <v>0.00347463222320292</v>
       </c>
       <c r="Q39" t="s">
         <v>23</v>
@@ -25512,40 +25512,40 @@
         <v>52</v>
       </c>
       <c r="E40" t="n">
-        <v>82016</v>
+        <v>64736</v>
       </c>
       <c r="F40" t="n">
-        <v>82016</v>
+        <v>54991</v>
       </c>
       <c r="G40" t="n">
-        <v>82016</v>
+        <v>53126</v>
       </c>
       <c r="H40" t="n">
-        <v>0.764618138424821</v>
+        <v>0.789309403043309</v>
       </c>
       <c r="I40" t="n">
-        <v>0.764760732535154</v>
+        <v>0.670491123683184</v>
       </c>
       <c r="J40" t="n">
-        <v>0.764618138424821</v>
+        <v>0.647751658213032</v>
       </c>
       <c r="K40" t="n">
-        <v>1309.15839613519</v>
+        <v>1210.94979765523</v>
       </c>
       <c r="L40" t="n">
-        <v>1309.15839613519</v>
+        <v>1240.6277659818</v>
       </c>
       <c r="M40" t="n">
-        <v>1309.15839613519</v>
+        <v>1208.74936924544</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.00931194669267898</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0113265843676149</v>
+        <v>0.0113234610137819</v>
       </c>
       <c r="P40" t="n">
-        <v>0.0112906000951926</v>
+        <v>0.0112307730915826</v>
       </c>
       <c r="Q40" t="s">
         <v>23</v>
@@ -26298,40 +26298,40 @@
         <v>52</v>
       </c>
       <c r="E53" t="n">
-        <v>18750</v>
+        <v>261602</v>
       </c>
       <c r="F53" t="n">
-        <v>6495</v>
+        <v>261577</v>
       </c>
       <c r="G53" t="n">
-        <v>5686</v>
+        <v>261602</v>
       </c>
       <c r="H53" t="n">
-        <v>0.0716737639620492</v>
+        <v>0.754537719386799</v>
       </c>
       <c r="I53" t="n">
-        <v>0.0248301647316087</v>
+        <v>0.754787812683051</v>
       </c>
       <c r="J53" t="n">
-        <v>0.021735307834038</v>
+        <v>0.754537719386799</v>
       </c>
       <c r="K53" t="n">
-        <v>1242.4073636488</v>
+        <v>2501.32257198692</v>
       </c>
       <c r="L53" t="n">
-        <v>809.74930757766</v>
+        <v>2500.28720132083</v>
       </c>
       <c r="M53" t="n">
-        <v>712.80851027292</v>
+        <v>2501.32257198692</v>
       </c>
       <c r="N53" t="n">
-        <v>0.00471669847814188</v>
+        <v>0.00644852439127255</v>
       </c>
       <c r="O53" t="n">
-        <v>0.00310336492896555</v>
+        <v>0.00649010549686331</v>
       </c>
       <c r="P53" t="n">
-        <v>0.0027395071922153</v>
+        <v>0.00644852439127255</v>
       </c>
       <c r="Q53" t="s">
         <v>23</v>
@@ -26360,40 +26360,40 @@
         <v>52</v>
       </c>
       <c r="E54" t="n">
-        <v>179301</v>
+        <v>18750</v>
       </c>
       <c r="F54" t="n">
-        <v>147690</v>
+        <v>6495</v>
       </c>
       <c r="G54" t="n">
-        <v>141989</v>
+        <v>5686</v>
       </c>
       <c r="H54" t="n">
-        <v>0.685396136115167</v>
+        <v>0.0716737639620492</v>
       </c>
       <c r="I54" t="n">
-        <v>0.564613861310436</v>
+        <v>0.0248301647316087</v>
       </c>
       <c r="J54" t="n">
-        <v>0.542767257131062</v>
+        <v>0.021735307834038</v>
       </c>
       <c r="K54" t="n">
-        <v>2122.68338987206</v>
+        <v>1242.4073636488</v>
       </c>
       <c r="L54" t="n">
-        <v>1811.25884655811</v>
+        <v>809.74930757766</v>
       </c>
       <c r="M54" t="n">
-        <v>1895.27634691521</v>
+        <v>712.80851027292</v>
       </c>
       <c r="N54" t="n">
-        <v>0.00612002931455315</v>
+        <v>0.00471669847814188</v>
       </c>
       <c r="O54" t="n">
-        <v>0.0053294207179917</v>
+        <v>0.00310336492896555</v>
       </c>
       <c r="P54" t="n">
-        <v>0.0061204535387096</v>
+        <v>0.0027395071922153</v>
       </c>
       <c r="Q54" t="s">
         <v>23</v>
@@ -26422,40 +26422,40 @@
         <v>52</v>
       </c>
       <c r="E55" t="n">
-        <v>261602</v>
+        <v>179301</v>
       </c>
       <c r="F55" t="n">
-        <v>261577</v>
+        <v>147690</v>
       </c>
       <c r="G55" t="n">
-        <v>261602</v>
+        <v>141989</v>
       </c>
       <c r="H55" t="n">
-        <v>0.754537719386799</v>
+        <v>0.685396136115167</v>
       </c>
       <c r="I55" t="n">
-        <v>0.754787812683051</v>
+        <v>0.564613861310436</v>
       </c>
       <c r="J55" t="n">
-        <v>0.754537719386799</v>
+        <v>0.542767257131062</v>
       </c>
       <c r="K55" t="n">
-        <v>2501.32257198692</v>
+        <v>2122.68338987206</v>
       </c>
       <c r="L55" t="n">
-        <v>2500.28720132083</v>
+        <v>1811.25884655811</v>
       </c>
       <c r="M55" t="n">
-        <v>2501.32257198692</v>
+        <v>1895.27634691521</v>
       </c>
       <c r="N55" t="n">
-        <v>0.00644852439127255</v>
+        <v>0.00612002931455315</v>
       </c>
       <c r="O55" t="n">
-        <v>0.00649010549686331</v>
+        <v>0.0053294207179917</v>
       </c>
       <c r="P55" t="n">
-        <v>0.00644852439127255</v>
+        <v>0.0061204535387096</v>
       </c>
       <c r="Q55" t="s">
         <v>23</v>
@@ -27208,40 +27208,40 @@
         <v>52</v>
       </c>
       <c r="E68" t="n">
-        <v>10890</v>
+        <v>239645</v>
       </c>
       <c r="F68" t="n">
-        <v>3969</v>
+        <v>239645</v>
       </c>
       <c r="G68" t="n">
-        <v>3691</v>
+        <v>239645</v>
       </c>
       <c r="H68" t="n">
-        <v>0.045442216612072</v>
+        <v>0.768519082696495</v>
       </c>
       <c r="I68" t="n">
-        <v>0.0165619979553089</v>
+        <v>0.76884701020873</v>
       </c>
       <c r="J68" t="n">
-        <v>0.0154019487158088</v>
+        <v>0.768519082696495</v>
       </c>
       <c r="K68" t="n">
-        <v>847.453087125624</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="L68" t="n">
-        <v>607.97428572679</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="M68" t="n">
-        <v>616.82608672745</v>
+        <v>2556.52132729956</v>
       </c>
       <c r="N68" t="n">
-        <v>0.00356500723312259</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="O68" t="n">
-        <v>0.002539866097422</v>
+        <v>0.00774704176324198</v>
       </c>
       <c r="P68" t="n">
-        <v>0.00257712385489421</v>
+        <v>0.00778311002667671</v>
       </c>
       <c r="Q68" t="s">
         <v>23</v>
@@ -27270,40 +27270,40 @@
         <v>52</v>
       </c>
       <c r="E69" t="n">
-        <v>166208</v>
+        <v>10890</v>
       </c>
       <c r="F69" t="n">
-        <v>141642</v>
+        <v>3969</v>
       </c>
       <c r="G69" t="n">
-        <v>136952</v>
+        <v>3691</v>
       </c>
       <c r="H69" t="n">
-        <v>0.69355922301738</v>
+        <v>0.045442216612072</v>
       </c>
       <c r="I69" t="n">
-        <v>0.591049260364289</v>
+        <v>0.0165619979553089</v>
       </c>
       <c r="J69" t="n">
-        <v>0.571478645496464</v>
+        <v>0.0154019487158088</v>
       </c>
       <c r="K69" t="n">
-        <v>2287.87585247375</v>
+        <v>847.453087125624</v>
       </c>
       <c r="L69" t="n">
-        <v>2107.858318533</v>
+        <v>607.97428572679</v>
       </c>
       <c r="M69" t="n">
-        <v>1957.33924894932</v>
+        <v>616.82608672745</v>
       </c>
       <c r="N69" t="n">
-        <v>0.00607006523918823</v>
+        <v>0.00356500723312259</v>
       </c>
       <c r="O69" t="n">
-        <v>0.00539918277279873</v>
+        <v>0.002539866097422</v>
       </c>
       <c r="P69" t="n">
-        <v>0.00555214543106352</v>
+        <v>0.00257712385489421</v>
       </c>
       <c r="Q69" t="s">
         <v>23</v>
@@ -27332,40 +27332,40 @@
         <v>52</v>
       </c>
       <c r="E70" t="n">
-        <v>239645</v>
+        <v>166208</v>
       </c>
       <c r="F70" t="n">
-        <v>239645</v>
+        <v>141642</v>
       </c>
       <c r="G70" t="n">
-        <v>239645</v>
+        <v>136952</v>
       </c>
       <c r="H70" t="n">
-        <v>0.768519082696495</v>
+        <v>0.69355922301738</v>
       </c>
       <c r="I70" t="n">
-        <v>0.76884701020873</v>
+        <v>0.591049260364289</v>
       </c>
       <c r="J70" t="n">
-        <v>0.768519082696495</v>
+        <v>0.571478645496464</v>
       </c>
       <c r="K70" t="n">
-        <v>2556.52132729956</v>
+        <v>2287.87585247375</v>
       </c>
       <c r="L70" t="n">
-        <v>2556.52132729956</v>
+        <v>2107.858318533</v>
       </c>
       <c r="M70" t="n">
-        <v>2556.52132729956</v>
+        <v>1957.33924894932</v>
       </c>
       <c r="N70" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.00607006523918823</v>
       </c>
       <c r="O70" t="n">
-        <v>0.00774704176324198</v>
+        <v>0.00539918277279873</v>
       </c>
       <c r="P70" t="n">
-        <v>0.00778311002667671</v>
+        <v>0.00555214543106352</v>
       </c>
       <c r="Q70" t="s">
         <v>23</v>

</xml_diff>